<commit_message>
Add servo damper support
Add servo damper support
Add checking of config file mtime to pitmaster to reduce load.
Add damper to wlt_2_nextion.py, display version need update, too.
</commit_message>
<xml_diff>
--- a/nextion/WLANThermo Nextion Variablentabelle.xlsx
+++ b/nextion/WLANThermo Nextion Variablentabelle.xlsx
@@ -468,9 +468,6 @@
     <t>nächste SSID nach "main.ssid.txt"</t>
   </si>
   <si>
-    <t>Ansteuerung FAN=0---- Servo=1 ----IO=2----IO PWM=3----Lüfter PWM=4</t>
-  </si>
-  <si>
     <t>pit_inverted</t>
   </si>
   <si>
@@ -727,6 +724,9 @@
   </si>
   <si>
     <t>Neues Logfile erstellen</t>
+  </si>
+  <si>
+    <t>Ansteuerung FAN=0---- Servo=1 ----IO=2----IO PWM=3----Lüfter PWM=4----Damper=5</t>
   </si>
 </sst>
 </file>
@@ -1611,6 +1611,7 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1627,7 +1628,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2812,8 +2812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV213"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A97" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="B140" sqref="B140"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -2853,7 +2853,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J1" s="44"/>
       <c r="K1" s="8"/>
@@ -2863,13 +2863,13 @@
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1">
       <c r="A2" s="9"/>
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="99"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="100"/>
       <c r="G2" s="50"/>
       <c r="H2" s="51"/>
       <c r="I2" s="51"/>
@@ -2884,7 +2884,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="64" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>9</v>
@@ -3124,13 +3124,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="64" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>11</v>
@@ -3144,7 +3144,7 @@
         <v>8</v>
       </c>
       <c r="J11" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
@@ -3156,13 +3156,13 @@
         <v>7</v>
       </c>
       <c r="B12" s="64" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>11</v>
@@ -3176,7 +3176,7 @@
         <v>8</v>
       </c>
       <c r="J12" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
@@ -3188,13 +3188,13 @@
         <v>7</v>
       </c>
       <c r="B13" s="64" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>11</v>
@@ -3208,7 +3208,7 @@
         <v>8</v>
       </c>
       <c r="J13" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
@@ -3220,13 +3220,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="64" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>11</v>
@@ -3240,7 +3240,7 @@
         <v>8</v>
       </c>
       <c r="J14" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
@@ -3252,7 +3252,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="64" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>9</v>
@@ -3286,7 +3286,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="64" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>9</v>
@@ -3796,13 +3796,13 @@
         <v>7</v>
       </c>
       <c r="B31" s="64" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>4</v>
@@ -3820,7 +3820,7 @@
         <v>5</v>
       </c>
       <c r="J31" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
@@ -3832,13 +3832,13 @@
         <v>7</v>
       </c>
       <c r="B32" s="64" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>4</v>
@@ -3856,7 +3856,7 @@
         <v>5</v>
       </c>
       <c r="J32" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
@@ -3868,13 +3868,13 @@
         <v>7</v>
       </c>
       <c r="B33" s="64" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>4</v>
@@ -3892,7 +3892,7 @@
         <v>5</v>
       </c>
       <c r="J33" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
@@ -3904,13 +3904,13 @@
         <v>7</v>
       </c>
       <c r="B34" s="64" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C34" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E34" s="11" t="s">
         <v>4</v>
@@ -3928,7 +3928,7 @@
         <v>5</v>
       </c>
       <c r="J34" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
@@ -3940,13 +3940,13 @@
         <v>7</v>
       </c>
       <c r="B35" s="64" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E35" s="11" t="s">
         <v>4</v>
@@ -3958,13 +3958,13 @@
         <v>0</v>
       </c>
       <c r="H35" s="55" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I35" s="55">
         <v>5</v>
       </c>
       <c r="J35" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
@@ -3976,13 +3976,13 @@
         <v>7</v>
       </c>
       <c r="B36" s="64" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>4</v>
@@ -3994,13 +3994,13 @@
         <v>1</v>
       </c>
       <c r="H36" s="55" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I36" s="55">
         <v>5</v>
       </c>
       <c r="J36" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
@@ -4012,13 +4012,13 @@
         <v>7</v>
       </c>
       <c r="B37" s="64" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C37" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E37" s="11" t="s">
         <v>4</v>
@@ -4030,13 +4030,13 @@
         <v>0</v>
       </c>
       <c r="H37" s="55" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I37" s="55">
         <v>5</v>
       </c>
       <c r="J37" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K37" s="8"/>
       <c r="L37" s="8"/>
@@ -4048,13 +4048,13 @@
         <v>7</v>
       </c>
       <c r="B38" s="64" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C38" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E38" s="11" t="s">
         <v>4</v>
@@ -4066,13 +4066,13 @@
         <v>1</v>
       </c>
       <c r="H38" s="55" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I38" s="55">
         <v>5</v>
       </c>
       <c r="J38" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
@@ -4084,7 +4084,7 @@
         <v>7</v>
       </c>
       <c r="B39" s="64" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>58</v>
@@ -4586,7 +4586,7 @@
         <v>9</v>
       </c>
       <c r="D55" s="64" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E55" s="11" t="s">
         <v>11</v>
@@ -4616,7 +4616,7 @@
         <v>9</v>
       </c>
       <c r="D56" s="64" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E56" s="11" t="s">
         <v>11</v>
@@ -4640,7 +4640,7 @@
         <v>7</v>
       </c>
       <c r="B57" s="65" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C57" s="41" t="s">
         <v>9</v>
@@ -4880,7 +4880,7 @@
         <v>7</v>
       </c>
       <c r="B65" s="65" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C65" s="43" t="s">
         <v>9</v>
@@ -4900,7 +4900,7 @@
         <v>10</v>
       </c>
       <c r="J65" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K65" s="8"/>
       <c r="L65" s="8"/>
@@ -4912,7 +4912,7 @@
         <v>7</v>
       </c>
       <c r="B66" s="65" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C66" s="43" t="s">
         <v>9</v>
@@ -4932,7 +4932,7 @@
         <v>10</v>
       </c>
       <c r="J66" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K66" s="8"/>
       <c r="L66" s="8"/>
@@ -4944,7 +4944,7 @@
         <v>7</v>
       </c>
       <c r="B67" s="65" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C67" s="43" t="s">
         <v>9</v>
@@ -4964,7 +4964,7 @@
         <v>10</v>
       </c>
       <c r="J67" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K67" s="8"/>
       <c r="L67" s="8"/>
@@ -4976,7 +4976,7 @@
         <v>7</v>
       </c>
       <c r="B68" s="65" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C68" s="43" t="s">
         <v>9</v>
@@ -4996,7 +4996,7 @@
         <v>10</v>
       </c>
       <c r="J68" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K68" s="8"/>
       <c r="L68" s="8"/>
@@ -5008,13 +5008,13 @@
         <v>7</v>
       </c>
       <c r="B69" s="73" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C69" s="76" t="s">
         <v>9</v>
       </c>
       <c r="D69" s="76" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E69" s="76" t="s">
         <v>11</v>
@@ -5038,13 +5038,13 @@
         <v>7</v>
       </c>
       <c r="B70" s="73" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C70" s="76" t="s">
         <v>9</v>
       </c>
       <c r="D70" s="76" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E70" s="76" t="s">
         <v>11</v>
@@ -5068,13 +5068,13 @@
         <v>7</v>
       </c>
       <c r="B71" s="73" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C71" s="76" t="s">
         <v>9</v>
       </c>
       <c r="D71" s="76" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E71" s="76" t="s">
         <v>11</v>
@@ -5098,13 +5098,13 @@
         <v>7</v>
       </c>
       <c r="B72" s="73" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C72" s="76" t="s">
         <v>9</v>
       </c>
       <c r="D72" s="76" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E72" s="76" t="s">
         <v>11</v>
@@ -5128,13 +5128,13 @@
         <v>7</v>
       </c>
       <c r="B73" s="73" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C73" s="76" t="s">
         <v>9</v>
       </c>
       <c r="D73" s="76" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E73" s="76" t="s">
         <v>11</v>
@@ -5158,13 +5158,13 @@
         <v>7</v>
       </c>
       <c r="B74" s="73" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C74" s="76" t="s">
         <v>9</v>
       </c>
       <c r="D74" s="76" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E74" s="76" t="s">
         <v>11</v>
@@ -5188,13 +5188,13 @@
         <v>7</v>
       </c>
       <c r="B75" s="73" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C75" s="76" t="s">
         <v>9</v>
       </c>
       <c r="D75" s="76" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E75" s="76" t="s">
         <v>11</v>
@@ -5218,13 +5218,13 @@
         <v>7</v>
       </c>
       <c r="B76" s="74" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C76" s="76" t="s">
         <v>9</v>
       </c>
       <c r="D76" s="76" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E76" s="76" t="s">
         <v>11</v>
@@ -5248,13 +5248,13 @@
         <v>7</v>
       </c>
       <c r="B77" s="74" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C77" s="76" t="s">
         <v>9</v>
       </c>
       <c r="D77" s="76" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E77" s="76" t="s">
         <v>11</v>
@@ -5268,7 +5268,7 @@
         <v>8</v>
       </c>
       <c r="J77" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K77" s="8"/>
       <c r="L77" s="8"/>
@@ -5280,13 +5280,13 @@
         <v>7</v>
       </c>
       <c r="B78" s="74" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C78" s="76" t="s">
         <v>9</v>
       </c>
       <c r="D78" s="76" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E78" s="76" t="s">
         <v>11</v>
@@ -5300,7 +5300,7 @@
         <v>8</v>
       </c>
       <c r="J78" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K78" s="8"/>
       <c r="L78" s="8"/>
@@ -5312,13 +5312,13 @@
         <v>7</v>
       </c>
       <c r="B79" s="76" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C79" s="76" t="s">
         <v>9</v>
       </c>
       <c r="D79" s="76" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E79" s="76" t="s">
         <v>11</v>
@@ -5332,7 +5332,7 @@
         <v>8</v>
       </c>
       <c r="J79" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K79" s="8"/>
       <c r="L79" s="8"/>
@@ -5344,13 +5344,13 @@
         <v>7</v>
       </c>
       <c r="B80" s="76" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C80" s="81" t="s">
         <v>9</v>
       </c>
       <c r="D80" s="76" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E80" s="76" t="s">
         <v>11</v>
@@ -5364,7 +5364,7 @@
         <v>8</v>
       </c>
       <c r="J80" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K80" s="8"/>
       <c r="L80" s="8"/>
@@ -5421,13 +5421,13 @@
     </row>
     <row r="84" spans="1:256" ht="15.75" customHeight="1">
       <c r="A84" s="20"/>
-      <c r="B84" s="92" t="s">
+      <c r="B84" s="93" t="s">
         <v>100</v>
       </c>
-      <c r="C84" s="93"/>
-      <c r="D84" s="93"/>
-      <c r="E84" s="93"/>
-      <c r="F84" s="94"/>
+      <c r="C84" s="94"/>
+      <c r="D84" s="94"/>
+      <c r="E84" s="94"/>
+      <c r="F84" s="95"/>
       <c r="G84" s="21"/>
       <c r="H84" s="22"/>
       <c r="I84" s="22"/>
@@ -5448,7 +5448,7 @@
         <v>58</v>
       </c>
       <c r="D85" s="87" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E85" s="11" t="s">
         <v>4</v>
@@ -5464,7 +5464,7 @@
       </c>
       <c r="I85" s="55"/>
       <c r="J85" s="44" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K85" s="8"/>
       <c r="L85" s="8"/>
@@ -5640,7 +5640,7 @@
         <v>58</v>
       </c>
       <c r="D91" s="67" t="s">
-        <v>150</v>
+        <v>236</v>
       </c>
       <c r="E91" s="67" t="s">
         <v>4</v>
@@ -5908,13 +5908,13 @@
         <v>7</v>
       </c>
       <c r="B92" s="67" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C92" s="67" t="s">
         <v>58</v>
       </c>
       <c r="D92" s="67" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E92" s="67" t="s">
         <v>4</v>
@@ -6182,13 +6182,13 @@
         <v>7</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C93" s="11" t="s">
         <v>58</v>
       </c>
       <c r="D93" s="87" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E93" s="11" t="s">
         <v>4</v>
@@ -6204,7 +6204,7 @@
       </c>
       <c r="I93" s="70"/>
       <c r="J93" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K93" s="44"/>
       <c r="L93" s="44"/>
@@ -6458,7 +6458,7 @@
         <v>7</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C94" s="11" t="s">
         <v>58</v>
@@ -6476,7 +6476,7 @@
       <c r="H94" s="53"/>
       <c r="I94" s="70"/>
       <c r="J94" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K94" s="44"/>
       <c r="L94" s="44"/>
@@ -6730,7 +6730,7 @@
         <v>7</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C95" s="11" t="s">
         <v>9</v>
@@ -6752,7 +6752,7 @@
       </c>
       <c r="I95" s="70"/>
       <c r="J95" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K95" s="44"/>
       <c r="L95" s="44"/>
@@ -7006,7 +7006,7 @@
         <v>7</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C96" s="11" t="s">
         <v>58</v>
@@ -7028,7 +7028,7 @@
       </c>
       <c r="I96" s="70"/>
       <c r="J96" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K96" s="44"/>
       <c r="L96" s="44"/>
@@ -7282,7 +7282,7 @@
         <v>7</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C97" s="11" t="s">
         <v>58</v>
@@ -7304,7 +7304,7 @@
       </c>
       <c r="I97" s="70"/>
       <c r="J97" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K97" s="44"/>
       <c r="L97" s="44"/>
@@ -7558,7 +7558,7 @@
         <v>7</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C98" s="11" t="s">
         <v>58</v>
@@ -7580,7 +7580,7 @@
       </c>
       <c r="I98" s="70"/>
       <c r="J98" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K98" s="44"/>
       <c r="L98" s="44"/>
@@ -7834,13 +7834,13 @@
         <v>7</v>
       </c>
       <c r="B99" s="67" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C99" s="67" t="s">
         <v>58</v>
       </c>
       <c r="D99" s="67" t="s">
-        <v>150</v>
+        <v>236</v>
       </c>
       <c r="E99" s="67" t="s">
         <v>4</v>
@@ -7856,7 +7856,7 @@
       </c>
       <c r="I99" s="70"/>
       <c r="J99" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K99" s="44"/>
       <c r="L99" s="44"/>
@@ -8110,13 +8110,13 @@
         <v>7</v>
       </c>
       <c r="B100" s="67" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C100" s="67" t="s">
         <v>58</v>
       </c>
       <c r="D100" s="67" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E100" s="67" t="s">
         <v>4</v>
@@ -8132,7 +8132,7 @@
       </c>
       <c r="I100" s="70"/>
       <c r="J100" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K100" s="44"/>
       <c r="L100" s="44"/>
@@ -8386,13 +8386,13 @@
         <v>7</v>
       </c>
       <c r="B101" s="67" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C101" s="67" t="s">
         <v>58</v>
       </c>
       <c r="D101" s="67" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E101" s="11" t="s">
         <v>11</v>
@@ -8404,7 +8404,7 @@
       <c r="H101" s="70"/>
       <c r="I101" s="70"/>
       <c r="J101" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K101" s="47"/>
       <c r="L101" s="47"/>
@@ -8687,13 +8687,13 @@
     </row>
     <row r="104" spans="1:256" ht="15.75" customHeight="1">
       <c r="A104" s="20"/>
-      <c r="B104" s="92" t="s">
+      <c r="B104" s="93" t="s">
         <v>113</v>
       </c>
-      <c r="C104" s="93"/>
-      <c r="D104" s="93"/>
-      <c r="E104" s="93"/>
-      <c r="F104" s="94"/>
+      <c r="C104" s="94"/>
+      <c r="D104" s="94"/>
+      <c r="E104" s="94"/>
+      <c r="F104" s="95"/>
       <c r="G104" s="21"/>
       <c r="H104" s="22"/>
       <c r="I104" s="22"/>
@@ -8708,13 +8708,13 @@
         <v>7</v>
       </c>
       <c r="B105" s="64" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C105" s="64" t="s">
         <v>9</v>
       </c>
       <c r="D105" s="64" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E105" s="64" t="s">
         <v>11</v>
@@ -8738,13 +8738,13 @@
         <v>7</v>
       </c>
       <c r="B106" s="64" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C106" s="64" t="s">
         <v>9</v>
       </c>
       <c r="D106" s="64" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E106" s="64" t="s">
         <v>116</v>
@@ -9064,13 +9064,13 @@
         <v>7</v>
       </c>
       <c r="B116" s="91" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C116" s="91" t="s">
         <v>58</v>
       </c>
       <c r="D116" s="91" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E116" s="43" t="s">
         <v>11</v>
@@ -9082,7 +9082,7 @@
       <c r="H116" s="57"/>
       <c r="I116" s="57"/>
       <c r="J116" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K116" s="8"/>
       <c r="L116" s="8"/>
@@ -9123,13 +9123,13 @@
     </row>
     <row r="119" spans="1:14" ht="15.75" customHeight="1">
       <c r="A119" s="20"/>
-      <c r="B119" s="92" t="s">
+      <c r="B119" s="93" t="s">
         <v>139</v>
       </c>
-      <c r="C119" s="93"/>
-      <c r="D119" s="93"/>
-      <c r="E119" s="93"/>
-      <c r="F119" s="94"/>
+      <c r="C119" s="94"/>
+      <c r="D119" s="94"/>
+      <c r="E119" s="94"/>
+      <c r="F119" s="95"/>
       <c r="G119" s="21"/>
       <c r="H119" s="22"/>
       <c r="I119" s="22"/>
@@ -9301,13 +9301,13 @@
     </row>
     <row r="128" spans="1:14" ht="15.75" customHeight="1">
       <c r="A128" s="20"/>
-      <c r="B128" s="92" t="s">
+      <c r="B128" s="93" t="s">
         <v>145</v>
       </c>
-      <c r="C128" s="93"/>
-      <c r="D128" s="93"/>
-      <c r="E128" s="93"/>
-      <c r="F128" s="94"/>
+      <c r="C128" s="94"/>
+      <c r="D128" s="94"/>
+      <c r="E128" s="94"/>
+      <c r="F128" s="95"/>
       <c r="G128" s="21"/>
       <c r="H128" s="21"/>
       <c r="I128" s="21" t="s">
@@ -9413,14 +9413,14 @@
       <c r="A132" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B132" s="100" t="s">
-        <v>235</v>
+      <c r="B132" s="92" t="s">
+        <v>234</v>
       </c>
       <c r="C132" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="D132" s="100" t="s">
-        <v>236</v>
+      <c r="D132" s="92" t="s">
+        <v>235</v>
       </c>
       <c r="E132" s="28"/>
       <c r="F132" s="28"/>
@@ -9444,13 +9444,13 @@
         <v>7</v>
       </c>
       <c r="B133" s="28" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C133" s="28" t="s">
         <v>58</v>
       </c>
       <c r="D133" s="28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E133" s="28"/>
       <c r="F133" s="28"/>

</xml_diff>

<commit_message>
Changes in Display firmware
- Restart log button
- Damper with single Pitmaster
</commit_message>
<xml_diff>
--- a/nextion/WLANThermo Nextion Variablentabelle.xlsx
+++ b/nextion/WLANThermo Nextion Variablentabelle.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bjoern\Documents\GitHub\WLANThermo_v2\nextion\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="12510"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="239">
   <si>
     <t>Seite</t>
   </si>
@@ -727,13 +732,19 @@
   </si>
   <si>
     <t>Ansteuerung FAN=0---- Servo=1 ----IO=2----IO PWM=3----Lüfter PWM=4----Damper=5</t>
+  </si>
+  <si>
+    <t>pit_damper</t>
+  </si>
+  <si>
+    <t>Damper möglich 0 oder 1. Default 0 wenn der Raspberry nichts übergibt.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1702,6 +1713,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2809,14 +2828,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IV213"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV214"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A97" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="1" customWidth="1"/>
@@ -2831,7 +2850,7 @@
     <col min="11" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2861,7 +2880,7 @@
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
     </row>
-    <row r="2" spans="1:14" ht="15" customHeight="1">
+    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="96" t="s">
         <v>6</v>
@@ -2879,7 +2898,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1">
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>7</v>
       </c>
@@ -2909,7 +2928,7 @@
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
     </row>
-    <row r="4" spans="1:14" ht="15" customHeight="1">
+    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
@@ -2939,7 +2958,7 @@
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
     </row>
-    <row r="5" spans="1:14" ht="15" customHeight="1">
+    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>7</v>
       </c>
@@ -2969,7 +2988,7 @@
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="1:14" ht="15" customHeight="1">
+    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
@@ -2999,7 +3018,7 @@
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
     </row>
-    <row r="7" spans="1:14" ht="15" customHeight="1">
+    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
@@ -3029,7 +3048,7 @@
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
     </row>
-    <row r="8" spans="1:14" ht="15" customHeight="1">
+    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>7</v>
       </c>
@@ -3059,7 +3078,7 @@
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
     </row>
-    <row r="9" spans="1:14" ht="15" customHeight="1">
+    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>7</v>
       </c>
@@ -3089,7 +3108,7 @@
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
     </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1">
+    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>7</v>
       </c>
@@ -3119,7 +3138,7 @@
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
     </row>
-    <row r="11" spans="1:14" ht="15" customHeight="1">
+    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>7</v>
       </c>
@@ -3151,7 +3170,7 @@
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
     </row>
-    <row r="12" spans="1:14" ht="15" customHeight="1">
+    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>7</v>
       </c>
@@ -3183,7 +3202,7 @@
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
     </row>
-    <row r="13" spans="1:14" ht="15" customHeight="1">
+    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>7</v>
       </c>
@@ -3215,7 +3234,7 @@
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
     </row>
-    <row r="14" spans="1:14" ht="15" customHeight="1">
+    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>7</v>
       </c>
@@ -3247,7 +3266,7 @@
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
     </row>
-    <row r="15" spans="1:14" ht="30" customHeight="1">
+    <row r="15" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>7</v>
       </c>
@@ -3281,7 +3300,7 @@
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
     </row>
-    <row r="16" spans="1:14" ht="30" customHeight="1">
+    <row r="16" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>7</v>
       </c>
@@ -3315,7 +3334,7 @@
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
     </row>
-    <row r="17" spans="1:14" ht="30" customHeight="1">
+    <row r="17" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>7</v>
       </c>
@@ -3349,7 +3368,7 @@
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
     </row>
-    <row r="18" spans="1:14" ht="30" customHeight="1">
+    <row r="18" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>7</v>
       </c>
@@ -3383,7 +3402,7 @@
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
     </row>
-    <row r="19" spans="1:14" ht="30" customHeight="1">
+    <row r="19" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>7</v>
       </c>
@@ -3417,7 +3436,7 @@
       <c r="M19" s="8"/>
       <c r="N19" s="8"/>
     </row>
-    <row r="20" spans="1:14" ht="30" customHeight="1">
+    <row r="20" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>7</v>
       </c>
@@ -3451,7 +3470,7 @@
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>
     </row>
-    <row r="21" spans="1:14" ht="30" customHeight="1">
+    <row r="21" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>7</v>
       </c>
@@ -3485,7 +3504,7 @@
       <c r="M21" s="8"/>
       <c r="N21" s="8"/>
     </row>
-    <row r="22" spans="1:14" ht="30" customHeight="1">
+    <row r="22" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>7</v>
       </c>
@@ -3519,7 +3538,7 @@
       <c r="M22" s="8"/>
       <c r="N22" s="8"/>
     </row>
-    <row r="23" spans="1:14" ht="30" customHeight="1">
+    <row r="23" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>7</v>
       </c>
@@ -3553,7 +3572,7 @@
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
     </row>
-    <row r="24" spans="1:14" ht="30" customHeight="1">
+    <row r="24" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>7</v>
       </c>
@@ -3587,7 +3606,7 @@
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
     </row>
-    <row r="25" spans="1:14" ht="30" customHeight="1">
+    <row r="25" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>7</v>
       </c>
@@ -3621,7 +3640,7 @@
       <c r="M25" s="8"/>
       <c r="N25" s="8"/>
     </row>
-    <row r="26" spans="1:14" ht="30" customHeight="1">
+    <row r="26" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>7</v>
       </c>
@@ -3655,7 +3674,7 @@
       <c r="M26" s="8"/>
       <c r="N26" s="8"/>
     </row>
-    <row r="27" spans="1:14" ht="30" customHeight="1">
+    <row r="27" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>7</v>
       </c>
@@ -3689,7 +3708,7 @@
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
     </row>
-    <row r="28" spans="1:14" ht="30" customHeight="1">
+    <row r="28" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>7</v>
       </c>
@@ -3723,7 +3742,7 @@
       <c r="M28" s="8"/>
       <c r="N28" s="8"/>
     </row>
-    <row r="29" spans="1:14" ht="30" customHeight="1">
+    <row r="29" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>7</v>
       </c>
@@ -3757,7 +3776,7 @@
       <c r="M29" s="8"/>
       <c r="N29" s="8"/>
     </row>
-    <row r="30" spans="1:14" ht="30" customHeight="1">
+    <row r="30" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>7</v>
       </c>
@@ -3791,7 +3810,7 @@
       <c r="M30" s="8"/>
       <c r="N30" s="8"/>
     </row>
-    <row r="31" spans="1:14" ht="30" customHeight="1">
+    <row r="31" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>7</v>
       </c>
@@ -3827,7 +3846,7 @@
       <c r="M31" s="8"/>
       <c r="N31" s="8"/>
     </row>
-    <row r="32" spans="1:14" ht="30" customHeight="1">
+    <row r="32" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>7</v>
       </c>
@@ -3863,7 +3882,7 @@
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
     </row>
-    <row r="33" spans="1:14" ht="30" customHeight="1">
+    <row r="33" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>7</v>
       </c>
@@ -3899,7 +3918,7 @@
       <c r="M33" s="8"/>
       <c r="N33" s="8"/>
     </row>
-    <row r="34" spans="1:14" ht="30" customHeight="1">
+    <row r="34" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>7</v>
       </c>
@@ -3935,7 +3954,7 @@
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
     </row>
-    <row r="35" spans="1:14" ht="30" customHeight="1">
+    <row r="35" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>7</v>
       </c>
@@ -3971,7 +3990,7 @@
       <c r="M35" s="8"/>
       <c r="N35" s="8"/>
     </row>
-    <row r="36" spans="1:14" ht="30" customHeight="1">
+    <row r="36" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>7</v>
       </c>
@@ -4007,7 +4026,7 @@
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
     </row>
-    <row r="37" spans="1:14" ht="30" customHeight="1">
+    <row r="37" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>7</v>
       </c>
@@ -4043,7 +4062,7 @@
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
     </row>
-    <row r="38" spans="1:14" ht="30" customHeight="1">
+    <row r="38" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>7</v>
       </c>
@@ -4079,7 +4098,7 @@
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
     </row>
-    <row r="39" spans="1:14" ht="30" customHeight="1">
+    <row r="39" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>7</v>
       </c>
@@ -4111,7 +4130,7 @@
       <c r="M39" s="8"/>
       <c r="N39" s="8"/>
     </row>
-    <row r="40" spans="1:14" ht="30" customHeight="1">
+    <row r="40" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>7</v>
       </c>
@@ -4143,7 +4162,7 @@
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
     </row>
-    <row r="41" spans="1:14" ht="30" customHeight="1">
+    <row r="41" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>7</v>
       </c>
@@ -4175,7 +4194,7 @@
       <c r="M41" s="8"/>
       <c r="N41" s="8"/>
     </row>
-    <row r="42" spans="1:14" ht="30" customHeight="1">
+    <row r="42" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>7</v>
       </c>
@@ -4207,7 +4226,7 @@
       <c r="M42" s="8"/>
       <c r="N42" s="8"/>
     </row>
-    <row r="43" spans="1:14" ht="30" customHeight="1">
+    <row r="43" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>7</v>
       </c>
@@ -4239,7 +4258,7 @@
       <c r="M43" s="8"/>
       <c r="N43" s="8"/>
     </row>
-    <row r="44" spans="1:14" ht="30" customHeight="1">
+    <row r="44" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>7</v>
       </c>
@@ -4271,7 +4290,7 @@
       <c r="M44" s="8"/>
       <c r="N44" s="8"/>
     </row>
-    <row r="45" spans="1:14" ht="30" customHeight="1">
+    <row r="45" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
         <v>7</v>
       </c>
@@ -4303,7 +4322,7 @@
       <c r="M45" s="8"/>
       <c r="N45" s="8"/>
     </row>
-    <row r="46" spans="1:14" ht="30" customHeight="1">
+    <row r="46" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>7</v>
       </c>
@@ -4335,7 +4354,7 @@
       <c r="M46" s="8"/>
       <c r="N46" s="8"/>
     </row>
-    <row r="47" spans="1:14" ht="30" customHeight="1">
+    <row r="47" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
         <v>7</v>
       </c>
@@ -4365,7 +4384,7 @@
       <c r="M47" s="8"/>
       <c r="N47" s="8"/>
     </row>
-    <row r="48" spans="1:14" ht="30" customHeight="1">
+    <row r="48" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>7</v>
       </c>
@@ -4395,7 +4414,7 @@
       <c r="M48" s="8"/>
       <c r="N48" s="8"/>
     </row>
-    <row r="49" spans="1:14" ht="30" customHeight="1">
+    <row r="49" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
         <v>7</v>
       </c>
@@ -4425,7 +4444,7 @@
       <c r="M49" s="8"/>
       <c r="N49" s="8"/>
     </row>
-    <row r="50" spans="1:14" ht="30" customHeight="1">
+    <row r="50" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>7</v>
       </c>
@@ -4455,7 +4474,7 @@
       <c r="M50" s="8"/>
       <c r="N50" s="8"/>
     </row>
-    <row r="51" spans="1:14" ht="30" customHeight="1">
+    <row r="51" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
         <v>7</v>
       </c>
@@ -4485,7 +4504,7 @@
       <c r="M51" s="8"/>
       <c r="N51" s="8"/>
     </row>
-    <row r="52" spans="1:14" ht="30" customHeight="1">
+    <row r="52" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>7</v>
       </c>
@@ -4515,7 +4534,7 @@
       <c r="M52" s="8"/>
       <c r="N52" s="8"/>
     </row>
-    <row r="53" spans="1:14" ht="30" customHeight="1">
+    <row r="53" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>7</v>
       </c>
@@ -4545,7 +4564,7 @@
       <c r="M53" s="8"/>
       <c r="N53" s="8"/>
     </row>
-    <row r="54" spans="1:14" ht="30" customHeight="1">
+    <row r="54" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>7</v>
       </c>
@@ -4575,7 +4594,7 @@
       <c r="M54" s="8"/>
       <c r="N54" s="8"/>
     </row>
-    <row r="55" spans="1:14" ht="30" customHeight="1">
+    <row r="55" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>7</v>
       </c>
@@ -4605,7 +4624,7 @@
       <c r="M55" s="8"/>
       <c r="N55" s="8"/>
     </row>
-    <row r="56" spans="1:14" ht="30" customHeight="1">
+    <row r="56" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
         <v>7</v>
       </c>
@@ -4635,7 +4654,7 @@
       <c r="M56" s="8"/>
       <c r="N56" s="8"/>
     </row>
-    <row r="57" spans="1:14" ht="27" customHeight="1">
+    <row r="57" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="40" t="s">
         <v>7</v>
       </c>
@@ -4665,7 +4684,7 @@
       <c r="M57" s="8"/>
       <c r="N57" s="8"/>
     </row>
-    <row r="58" spans="1:14" ht="27" customHeight="1">
+    <row r="58" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="43" t="s">
         <v>7</v>
       </c>
@@ -4695,7 +4714,7 @@
       <c r="M58" s="8"/>
       <c r="N58" s="8"/>
     </row>
-    <row r="59" spans="1:14" ht="27" customHeight="1">
+    <row r="59" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="43" t="s">
         <v>7</v>
       </c>
@@ -4725,7 +4744,7 @@
       <c r="M59" s="8"/>
       <c r="N59" s="8"/>
     </row>
-    <row r="60" spans="1:14" ht="27.6" customHeight="1">
+    <row r="60" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="43" t="s">
         <v>7</v>
       </c>
@@ -4755,7 +4774,7 @@
       <c r="M60" s="8"/>
       <c r="N60" s="8"/>
     </row>
-    <row r="61" spans="1:14" ht="27.6" customHeight="1">
+    <row r="61" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="43" t="s">
         <v>7</v>
       </c>
@@ -4785,7 +4804,7 @@
       <c r="M61" s="8"/>
       <c r="N61" s="8"/>
     </row>
-    <row r="62" spans="1:14" ht="27.6" customHeight="1">
+    <row r="62" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="43" t="s">
         <v>7</v>
       </c>
@@ -4815,7 +4834,7 @@
       <c r="M62" s="8"/>
       <c r="N62" s="8"/>
     </row>
-    <row r="63" spans="1:14" ht="27.6" customHeight="1">
+    <row r="63" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="43" t="s">
         <v>7</v>
       </c>
@@ -4845,7 +4864,7 @@
       <c r="M63" s="8"/>
       <c r="N63" s="8"/>
     </row>
-    <row r="64" spans="1:14" ht="27.6" customHeight="1">
+    <row r="64" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="43" t="s">
         <v>7</v>
       </c>
@@ -4875,7 +4894,7 @@
       <c r="M64" s="8"/>
       <c r="N64" s="8"/>
     </row>
-    <row r="65" spans="1:14" ht="27.6" customHeight="1">
+    <row r="65" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="43" t="s">
         <v>7</v>
       </c>
@@ -4907,7 +4926,7 @@
       <c r="M65" s="8"/>
       <c r="N65" s="8"/>
     </row>
-    <row r="66" spans="1:14" ht="27.6" customHeight="1">
+    <row r="66" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="43" t="s">
         <v>7</v>
       </c>
@@ -4939,7 +4958,7 @@
       <c r="M66" s="8"/>
       <c r="N66" s="8"/>
     </row>
-    <row r="67" spans="1:14" ht="27.6" customHeight="1">
+    <row r="67" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="43" t="s">
         <v>7</v>
       </c>
@@ -4971,7 +4990,7 @@
       <c r="M67" s="8"/>
       <c r="N67" s="8"/>
     </row>
-    <row r="68" spans="1:14" ht="27.6" customHeight="1">
+    <row r="68" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="43" t="s">
         <v>7</v>
       </c>
@@ -5003,7 +5022,7 @@
       <c r="M68" s="8"/>
       <c r="N68" s="8"/>
     </row>
-    <row r="69" spans="1:14" ht="27" customHeight="1">
+    <row r="69" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="76" t="s">
         <v>7</v>
       </c>
@@ -5033,7 +5052,7 @@
       <c r="M69" s="8"/>
       <c r="N69" s="8"/>
     </row>
-    <row r="70" spans="1:14" ht="27" customHeight="1">
+    <row r="70" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="76" t="s">
         <v>7</v>
       </c>
@@ -5063,7 +5082,7 @@
       <c r="M70" s="8"/>
       <c r="N70" s="8"/>
     </row>
-    <row r="71" spans="1:14" ht="27" customHeight="1">
+    <row r="71" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="76" t="s">
         <v>7</v>
       </c>
@@ -5093,7 +5112,7 @@
       <c r="M71" s="8"/>
       <c r="N71" s="8"/>
     </row>
-    <row r="72" spans="1:14" ht="27" customHeight="1">
+    <row r="72" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="76" t="s">
         <v>7</v>
       </c>
@@ -5123,7 +5142,7 @@
       <c r="M72" s="8"/>
       <c r="N72" s="8"/>
     </row>
-    <row r="73" spans="1:14" ht="27" customHeight="1">
+    <row r="73" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="76" t="s">
         <v>7</v>
       </c>
@@ -5153,7 +5172,7 @@
       <c r="M73" s="8"/>
       <c r="N73" s="8"/>
     </row>
-    <row r="74" spans="1:14" ht="27" customHeight="1">
+    <row r="74" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="76" t="s">
         <v>7</v>
       </c>
@@ -5183,7 +5202,7 @@
       <c r="M74" s="8"/>
       <c r="N74" s="8"/>
     </row>
-    <row r="75" spans="1:14" ht="27" customHeight="1">
+    <row r="75" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="76" t="s">
         <v>7</v>
       </c>
@@ -5213,7 +5232,7 @@
       <c r="M75" s="8"/>
       <c r="N75" s="8"/>
     </row>
-    <row r="76" spans="1:14" ht="27" customHeight="1">
+    <row r="76" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="76" t="s">
         <v>7</v>
       </c>
@@ -5243,7 +5262,7 @@
       <c r="M76" s="8"/>
       <c r="N76" s="8"/>
     </row>
-    <row r="77" spans="1:14" ht="27" customHeight="1">
+    <row r="77" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="76" t="s">
         <v>7</v>
       </c>
@@ -5275,7 +5294,7 @@
       <c r="M77" s="8"/>
       <c r="N77" s="8"/>
     </row>
-    <row r="78" spans="1:14" ht="27" customHeight="1">
+    <row r="78" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="76" t="s">
         <v>7</v>
       </c>
@@ -5307,7 +5326,7 @@
       <c r="M78" s="8"/>
       <c r="N78" s="8"/>
     </row>
-    <row r="79" spans="1:14" ht="27" customHeight="1">
+    <row r="79" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="76" t="s">
         <v>7</v>
       </c>
@@ -5339,7 +5358,7 @@
       <c r="M79" s="8"/>
       <c r="N79" s="8"/>
     </row>
-    <row r="80" spans="1:14" ht="27" customHeight="1">
+    <row r="80" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="80" t="s">
         <v>7</v>
       </c>
@@ -5371,7 +5390,7 @@
       <c r="M80" s="8"/>
       <c r="N80" s="8"/>
     </row>
-    <row r="81" spans="1:256" ht="15.75" customHeight="1" thickBot="1">
+    <row r="81" spans="1:256" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="82"/>
       <c r="B81" s="83"/>
       <c r="C81" s="84"/>
@@ -5387,7 +5406,7 @@
       <c r="M81" s="8"/>
       <c r="N81" s="8"/>
     </row>
-    <row r="82" spans="1:256" ht="15" customHeight="1">
+    <row r="82" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="16"/>
       <c r="B82" s="16"/>
       <c r="C82" s="16"/>
@@ -5403,7 +5422,7 @@
       <c r="M82" s="8"/>
       <c r="N82" s="8"/>
     </row>
-    <row r="83" spans="1:256" ht="15.75" customHeight="1" thickBot="1">
+    <row r="83" spans="1:256" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="19"/>
       <c r="B83" s="19"/>
       <c r="C83" s="19"/>
@@ -5419,7 +5438,7 @@
       <c r="M83" s="8"/>
       <c r="N83" s="8"/>
     </row>
-    <row r="84" spans="1:256" ht="15.75" customHeight="1">
+    <row r="84" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="20"/>
       <c r="B84" s="93" t="s">
         <v>100</v>
@@ -5437,7 +5456,7 @@
       <c r="M84" s="8"/>
       <c r="N84" s="8"/>
     </row>
-    <row r="85" spans="1:256" ht="30" customHeight="1">
+    <row r="85" spans="1:256" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
         <v>7</v>
       </c>
@@ -5471,7 +5490,7 @@
       <c r="M85" s="8"/>
       <c r="N85" s="8"/>
     </row>
-    <row r="86" spans="1:256" ht="15" customHeight="1">
+    <row r="86" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
         <v>7</v>
       </c>
@@ -5499,7 +5518,7 @@
       <c r="M86" s="8"/>
       <c r="N86" s="8"/>
     </row>
-    <row r="87" spans="1:256" ht="30" customHeight="1">
+    <row r="87" spans="1:256" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="s">
         <v>7</v>
       </c>
@@ -5533,7 +5552,7 @@
       <c r="M87" s="8"/>
       <c r="N87" s="8"/>
     </row>
-    <row r="88" spans="1:256" ht="30" customHeight="1">
+    <row r="88" spans="1:256" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
         <v>7</v>
       </c>
@@ -5565,7 +5584,7 @@
       <c r="M88" s="8"/>
       <c r="N88" s="8"/>
     </row>
-    <row r="89" spans="1:256" ht="30" customHeight="1">
+    <row r="89" spans="1:256" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="10" t="s">
         <v>7</v>
       </c>
@@ -5597,7 +5616,7 @@
       <c r="M89" s="8"/>
       <c r="N89" s="8"/>
     </row>
-    <row r="90" spans="1:256" ht="30" customHeight="1">
+    <row r="90" spans="1:256" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="10" t="s">
         <v>7</v>
       </c>
@@ -5629,7 +5648,7 @@
       <c r="M90" s="8"/>
       <c r="N90" s="8"/>
     </row>
-    <row r="91" spans="1:256" s="46" customFormat="1" ht="30" customHeight="1">
+    <row r="91" spans="1:256" s="46" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="66" t="s">
         <v>7</v>
       </c>
@@ -5903,7 +5922,7 @@
       <c r="IU91" s="45"/>
       <c r="IV91" s="45"/>
     </row>
-    <row r="92" spans="1:256" s="46" customFormat="1" ht="30" customHeight="1">
+    <row r="92" spans="1:256" s="46" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="66" t="s">
         <v>7</v>
       </c>
@@ -6177,7 +6196,7 @@
       <c r="IU92" s="45"/>
       <c r="IV92" s="45"/>
     </row>
-    <row r="93" spans="1:256" s="46" customFormat="1" ht="30" customHeight="1">
+    <row r="93" spans="1:256" s="46" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="10" t="s">
         <v>7</v>
       </c>
@@ -6453,7 +6472,7 @@
       <c r="IU93" s="45"/>
       <c r="IV93" s="45"/>
     </row>
-    <row r="94" spans="1:256" s="46" customFormat="1" ht="30" customHeight="1">
+    <row r="94" spans="1:256" s="46" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="10" t="s">
         <v>7</v>
       </c>
@@ -6725,7 +6744,7 @@
       <c r="IU94" s="45"/>
       <c r="IV94" s="45"/>
     </row>
-    <row r="95" spans="1:256" s="46" customFormat="1" ht="30" customHeight="1">
+    <row r="95" spans="1:256" s="46" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="10" t="s">
         <v>7</v>
       </c>
@@ -7001,7 +7020,7 @@
       <c r="IU95" s="45"/>
       <c r="IV95" s="45"/>
     </row>
-    <row r="96" spans="1:256" s="46" customFormat="1" ht="30" customHeight="1">
+    <row r="96" spans="1:256" s="46" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="s">
         <v>7</v>
       </c>
@@ -7277,7 +7296,7 @@
       <c r="IU96" s="45"/>
       <c r="IV96" s="45"/>
     </row>
-    <row r="97" spans="1:256" s="46" customFormat="1" ht="30" customHeight="1">
+    <row r="97" spans="1:256" s="46" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="s">
         <v>7</v>
       </c>
@@ -7553,7 +7572,7 @@
       <c r="IU97" s="45"/>
       <c r="IV97" s="45"/>
     </row>
-    <row r="98" spans="1:256" s="46" customFormat="1" ht="30" customHeight="1">
+    <row r="98" spans="1:256" s="46" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="10" t="s">
         <v>7</v>
       </c>
@@ -7829,7 +7848,7 @@
       <c r="IU98" s="45"/>
       <c r="IV98" s="45"/>
     </row>
-    <row r="99" spans="1:256" s="46" customFormat="1" ht="30" customHeight="1">
+    <row r="99" spans="1:256" s="46" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="66" t="s">
         <v>7</v>
       </c>
@@ -8105,7 +8124,7 @@
       <c r="IU99" s="45"/>
       <c r="IV99" s="45"/>
     </row>
-    <row r="100" spans="1:256" s="46" customFormat="1" ht="30" customHeight="1">
+    <row r="100" spans="1:256" s="46" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="66" t="s">
         <v>7</v>
       </c>
@@ -8381,7 +8400,7 @@
       <c r="IU100" s="45"/>
       <c r="IV100" s="45"/>
     </row>
-    <row r="101" spans="1:256" s="49" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="101" spans="1:256" s="46" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="66" t="s">
         <v>7</v>
       </c>
@@ -8406,356 +8425,598 @@
       <c r="J101" s="44" t="s">
         <v>190</v>
       </c>
-      <c r="K101" s="47"/>
-      <c r="L101" s="47"/>
-      <c r="M101" s="47"/>
-      <c r="N101" s="47"/>
-      <c r="O101" s="48"/>
-      <c r="P101" s="48"/>
-      <c r="Q101" s="48"/>
-      <c r="R101" s="48"/>
-      <c r="S101" s="48"/>
-      <c r="T101" s="48"/>
-      <c r="U101" s="48"/>
-      <c r="V101" s="48"/>
-      <c r="W101" s="48"/>
-      <c r="X101" s="48"/>
-      <c r="Y101" s="48"/>
-      <c r="Z101" s="48"/>
-      <c r="AA101" s="48"/>
-      <c r="AB101" s="48"/>
-      <c r="AC101" s="48"/>
-      <c r="AD101" s="48"/>
-      <c r="AE101" s="48"/>
-      <c r="AF101" s="48"/>
-      <c r="AG101" s="48"/>
-      <c r="AH101" s="48"/>
-      <c r="AI101" s="48"/>
-      <c r="AJ101" s="48"/>
-      <c r="AK101" s="48"/>
-      <c r="AL101" s="48"/>
-      <c r="AM101" s="48"/>
-      <c r="AN101" s="48"/>
-      <c r="AO101" s="48"/>
-      <c r="AP101" s="48"/>
-      <c r="AQ101" s="48"/>
-      <c r="AR101" s="48"/>
-      <c r="AS101" s="48"/>
-      <c r="AT101" s="48"/>
-      <c r="AU101" s="48"/>
-      <c r="AV101" s="48"/>
-      <c r="AW101" s="48"/>
-      <c r="AX101" s="48"/>
-      <c r="AY101" s="48"/>
-      <c r="AZ101" s="48"/>
-      <c r="BA101" s="48"/>
-      <c r="BB101" s="48"/>
-      <c r="BC101" s="48"/>
-      <c r="BD101" s="48"/>
-      <c r="BE101" s="48"/>
-      <c r="BF101" s="48"/>
-      <c r="BG101" s="48"/>
-      <c r="BH101" s="48"/>
-      <c r="BI101" s="48"/>
-      <c r="BJ101" s="48"/>
-      <c r="BK101" s="48"/>
-      <c r="BL101" s="48"/>
-      <c r="BM101" s="48"/>
-      <c r="BN101" s="48"/>
-      <c r="BO101" s="48"/>
-      <c r="BP101" s="48"/>
-      <c r="BQ101" s="48"/>
-      <c r="BR101" s="48"/>
-      <c r="BS101" s="48"/>
-      <c r="BT101" s="48"/>
-      <c r="BU101" s="48"/>
-      <c r="BV101" s="48"/>
-      <c r="BW101" s="48"/>
-      <c r="BX101" s="48"/>
-      <c r="BY101" s="48"/>
-      <c r="BZ101" s="48"/>
-      <c r="CA101" s="48"/>
-      <c r="CB101" s="48"/>
-      <c r="CC101" s="48"/>
-      <c r="CD101" s="48"/>
-      <c r="CE101" s="48"/>
-      <c r="CF101" s="48"/>
-      <c r="CG101" s="48"/>
-      <c r="CH101" s="48"/>
-      <c r="CI101" s="48"/>
-      <c r="CJ101" s="48"/>
-      <c r="CK101" s="48"/>
-      <c r="CL101" s="48"/>
-      <c r="CM101" s="48"/>
-      <c r="CN101" s="48"/>
-      <c r="CO101" s="48"/>
-      <c r="CP101" s="48"/>
-      <c r="CQ101" s="48"/>
-      <c r="CR101" s="48"/>
-      <c r="CS101" s="48"/>
-      <c r="CT101" s="48"/>
-      <c r="CU101" s="48"/>
-      <c r="CV101" s="48"/>
-      <c r="CW101" s="48"/>
-      <c r="CX101" s="48"/>
-      <c r="CY101" s="48"/>
-      <c r="CZ101" s="48"/>
-      <c r="DA101" s="48"/>
-      <c r="DB101" s="48"/>
-      <c r="DC101" s="48"/>
-      <c r="DD101" s="48"/>
-      <c r="DE101" s="48"/>
-      <c r="DF101" s="48"/>
-      <c r="DG101" s="48"/>
-      <c r="DH101" s="48"/>
-      <c r="DI101" s="48"/>
-      <c r="DJ101" s="48"/>
-      <c r="DK101" s="48"/>
-      <c r="DL101" s="48"/>
-      <c r="DM101" s="48"/>
-      <c r="DN101" s="48"/>
-      <c r="DO101" s="48"/>
-      <c r="DP101" s="48"/>
-      <c r="DQ101" s="48"/>
-      <c r="DR101" s="48"/>
-      <c r="DS101" s="48"/>
-      <c r="DT101" s="48"/>
-      <c r="DU101" s="48"/>
-      <c r="DV101" s="48"/>
-      <c r="DW101" s="48"/>
-      <c r="DX101" s="48"/>
-      <c r="DY101" s="48"/>
-      <c r="DZ101" s="48"/>
-      <c r="EA101" s="48"/>
-      <c r="EB101" s="48"/>
-      <c r="EC101" s="48"/>
-      <c r="ED101" s="48"/>
-      <c r="EE101" s="48"/>
-      <c r="EF101" s="48"/>
-      <c r="EG101" s="48"/>
-      <c r="EH101" s="48"/>
-      <c r="EI101" s="48"/>
-      <c r="EJ101" s="48"/>
-      <c r="EK101" s="48"/>
-      <c r="EL101" s="48"/>
-      <c r="EM101" s="48"/>
-      <c r="EN101" s="48"/>
-      <c r="EO101" s="48"/>
-      <c r="EP101" s="48"/>
-      <c r="EQ101" s="48"/>
-      <c r="ER101" s="48"/>
-      <c r="ES101" s="48"/>
-      <c r="ET101" s="48"/>
-      <c r="EU101" s="48"/>
-      <c r="EV101" s="48"/>
-      <c r="EW101" s="48"/>
-      <c r="EX101" s="48"/>
-      <c r="EY101" s="48"/>
-      <c r="EZ101" s="48"/>
-      <c r="FA101" s="48"/>
-      <c r="FB101" s="48"/>
-      <c r="FC101" s="48"/>
-      <c r="FD101" s="48"/>
-      <c r="FE101" s="48"/>
-      <c r="FF101" s="48"/>
-      <c r="FG101" s="48"/>
-      <c r="FH101" s="48"/>
-      <c r="FI101" s="48"/>
-      <c r="FJ101" s="48"/>
-      <c r="FK101" s="48"/>
-      <c r="FL101" s="48"/>
-      <c r="FM101" s="48"/>
-      <c r="FN101" s="48"/>
-      <c r="FO101" s="48"/>
-      <c r="FP101" s="48"/>
-      <c r="FQ101" s="48"/>
-      <c r="FR101" s="48"/>
-      <c r="FS101" s="48"/>
-      <c r="FT101" s="48"/>
-      <c r="FU101" s="48"/>
-      <c r="FV101" s="48"/>
-      <c r="FW101" s="48"/>
-      <c r="FX101" s="48"/>
-      <c r="FY101" s="48"/>
-      <c r="FZ101" s="48"/>
-      <c r="GA101" s="48"/>
-      <c r="GB101" s="48"/>
-      <c r="GC101" s="48"/>
-      <c r="GD101" s="48"/>
-      <c r="GE101" s="48"/>
-      <c r="GF101" s="48"/>
-      <c r="GG101" s="48"/>
-      <c r="GH101" s="48"/>
-      <c r="GI101" s="48"/>
-      <c r="GJ101" s="48"/>
-      <c r="GK101" s="48"/>
-      <c r="GL101" s="48"/>
-      <c r="GM101" s="48"/>
-      <c r="GN101" s="48"/>
-      <c r="GO101" s="48"/>
-      <c r="GP101" s="48"/>
-      <c r="GQ101" s="48"/>
-      <c r="GR101" s="48"/>
-      <c r="GS101" s="48"/>
-      <c r="GT101" s="48"/>
-      <c r="GU101" s="48"/>
-      <c r="GV101" s="48"/>
-      <c r="GW101" s="48"/>
-      <c r="GX101" s="48"/>
-      <c r="GY101" s="48"/>
-      <c r="GZ101" s="48"/>
-      <c r="HA101" s="48"/>
-      <c r="HB101" s="48"/>
-      <c r="HC101" s="48"/>
-      <c r="HD101" s="48"/>
-      <c r="HE101" s="48"/>
-      <c r="HF101" s="48"/>
-      <c r="HG101" s="48"/>
-      <c r="HH101" s="48"/>
-      <c r="HI101" s="48"/>
-      <c r="HJ101" s="48"/>
-      <c r="HK101" s="48"/>
-      <c r="HL101" s="48"/>
-      <c r="HM101" s="48"/>
-      <c r="HN101" s="48"/>
-      <c r="HO101" s="48"/>
-      <c r="HP101" s="48"/>
-      <c r="HQ101" s="48"/>
-      <c r="HR101" s="48"/>
-      <c r="HS101" s="48"/>
-      <c r="HT101" s="48"/>
-      <c r="HU101" s="48"/>
-      <c r="HV101" s="48"/>
-      <c r="HW101" s="48"/>
-      <c r="HX101" s="48"/>
-      <c r="HY101" s="48"/>
-      <c r="HZ101" s="48"/>
-      <c r="IA101" s="48"/>
-      <c r="IB101" s="48"/>
-      <c r="IC101" s="48"/>
-      <c r="ID101" s="48"/>
-      <c r="IE101" s="48"/>
-      <c r="IF101" s="48"/>
-      <c r="IG101" s="48"/>
-      <c r="IH101" s="48"/>
-      <c r="II101" s="48"/>
-      <c r="IJ101" s="48"/>
-      <c r="IK101" s="48"/>
-      <c r="IL101" s="48"/>
-      <c r="IM101" s="48"/>
-      <c r="IN101" s="48"/>
-      <c r="IO101" s="48"/>
-      <c r="IP101" s="48"/>
-      <c r="IQ101" s="48"/>
-      <c r="IR101" s="48"/>
-      <c r="IS101" s="48"/>
-      <c r="IT101" s="48"/>
-      <c r="IU101" s="48"/>
-      <c r="IV101" s="48"/>
-    </row>
-    <row r="102" spans="1:256" ht="15" customHeight="1">
-      <c r="A102" s="16"/>
-      <c r="B102" s="16"/>
-      <c r="C102" s="16"/>
-      <c r="D102" s="16"/>
-      <c r="E102" s="16"/>
-      <c r="F102" s="16"/>
-      <c r="G102" s="58"/>
-      <c r="H102" s="59"/>
-      <c r="I102" s="59"/>
-      <c r="J102" s="44"/>
-      <c r="K102" s="8"/>
-      <c r="L102" s="8"/>
-      <c r="M102" s="8"/>
-      <c r="N102" s="8"/>
-    </row>
-    <row r="103" spans="1:256" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A103" s="19"/>
-      <c r="B103" s="19"/>
-      <c r="C103" s="19"/>
-      <c r="D103" s="19"/>
-      <c r="E103" s="19"/>
-      <c r="F103" s="19"/>
-      <c r="G103" s="60"/>
-      <c r="H103" s="61"/>
-      <c r="I103" s="61"/>
+      <c r="K101" s="44"/>
+      <c r="L101" s="44"/>
+      <c r="M101" s="44"/>
+      <c r="N101" s="44"/>
+      <c r="O101" s="45"/>
+      <c r="P101" s="45"/>
+      <c r="Q101" s="45"/>
+      <c r="R101" s="45"/>
+      <c r="S101" s="45"/>
+      <c r="T101" s="45"/>
+      <c r="U101" s="45"/>
+      <c r="V101" s="45"/>
+      <c r="W101" s="45"/>
+      <c r="X101" s="45"/>
+      <c r="Y101" s="45"/>
+      <c r="Z101" s="45"/>
+      <c r="AA101" s="45"/>
+      <c r="AB101" s="45"/>
+      <c r="AC101" s="45"/>
+      <c r="AD101" s="45"/>
+      <c r="AE101" s="45"/>
+      <c r="AF101" s="45"/>
+      <c r="AG101" s="45"/>
+      <c r="AH101" s="45"/>
+      <c r="AI101" s="45"/>
+      <c r="AJ101" s="45"/>
+      <c r="AK101" s="45"/>
+      <c r="AL101" s="45"/>
+      <c r="AM101" s="45"/>
+      <c r="AN101" s="45"/>
+      <c r="AO101" s="45"/>
+      <c r="AP101" s="45"/>
+      <c r="AQ101" s="45"/>
+      <c r="AR101" s="45"/>
+      <c r="AS101" s="45"/>
+      <c r="AT101" s="45"/>
+      <c r="AU101" s="45"/>
+      <c r="AV101" s="45"/>
+      <c r="AW101" s="45"/>
+      <c r="AX101" s="45"/>
+      <c r="AY101" s="45"/>
+      <c r="AZ101" s="45"/>
+      <c r="BA101" s="45"/>
+      <c r="BB101" s="45"/>
+      <c r="BC101" s="45"/>
+      <c r="BD101" s="45"/>
+      <c r="BE101" s="45"/>
+      <c r="BF101" s="45"/>
+      <c r="BG101" s="45"/>
+      <c r="BH101" s="45"/>
+      <c r="BI101" s="45"/>
+      <c r="BJ101" s="45"/>
+      <c r="BK101" s="45"/>
+      <c r="BL101" s="45"/>
+      <c r="BM101" s="45"/>
+      <c r="BN101" s="45"/>
+      <c r="BO101" s="45"/>
+      <c r="BP101" s="45"/>
+      <c r="BQ101" s="45"/>
+      <c r="BR101" s="45"/>
+      <c r="BS101" s="45"/>
+      <c r="BT101" s="45"/>
+      <c r="BU101" s="45"/>
+      <c r="BV101" s="45"/>
+      <c r="BW101" s="45"/>
+      <c r="BX101" s="45"/>
+      <c r="BY101" s="45"/>
+      <c r="BZ101" s="45"/>
+      <c r="CA101" s="45"/>
+      <c r="CB101" s="45"/>
+      <c r="CC101" s="45"/>
+      <c r="CD101" s="45"/>
+      <c r="CE101" s="45"/>
+      <c r="CF101" s="45"/>
+      <c r="CG101" s="45"/>
+      <c r="CH101" s="45"/>
+      <c r="CI101" s="45"/>
+      <c r="CJ101" s="45"/>
+      <c r="CK101" s="45"/>
+      <c r="CL101" s="45"/>
+      <c r="CM101" s="45"/>
+      <c r="CN101" s="45"/>
+      <c r="CO101" s="45"/>
+      <c r="CP101" s="45"/>
+      <c r="CQ101" s="45"/>
+      <c r="CR101" s="45"/>
+      <c r="CS101" s="45"/>
+      <c r="CT101" s="45"/>
+      <c r="CU101" s="45"/>
+      <c r="CV101" s="45"/>
+      <c r="CW101" s="45"/>
+      <c r="CX101" s="45"/>
+      <c r="CY101" s="45"/>
+      <c r="CZ101" s="45"/>
+      <c r="DA101" s="45"/>
+      <c r="DB101" s="45"/>
+      <c r="DC101" s="45"/>
+      <c r="DD101" s="45"/>
+      <c r="DE101" s="45"/>
+      <c r="DF101" s="45"/>
+      <c r="DG101" s="45"/>
+      <c r="DH101" s="45"/>
+      <c r="DI101" s="45"/>
+      <c r="DJ101" s="45"/>
+      <c r="DK101" s="45"/>
+      <c r="DL101" s="45"/>
+      <c r="DM101" s="45"/>
+      <c r="DN101" s="45"/>
+      <c r="DO101" s="45"/>
+      <c r="DP101" s="45"/>
+      <c r="DQ101" s="45"/>
+      <c r="DR101" s="45"/>
+      <c r="DS101" s="45"/>
+      <c r="DT101" s="45"/>
+      <c r="DU101" s="45"/>
+      <c r="DV101" s="45"/>
+      <c r="DW101" s="45"/>
+      <c r="DX101" s="45"/>
+      <c r="DY101" s="45"/>
+      <c r="DZ101" s="45"/>
+      <c r="EA101" s="45"/>
+      <c r="EB101" s="45"/>
+      <c r="EC101" s="45"/>
+      <c r="ED101" s="45"/>
+      <c r="EE101" s="45"/>
+      <c r="EF101" s="45"/>
+      <c r="EG101" s="45"/>
+      <c r="EH101" s="45"/>
+      <c r="EI101" s="45"/>
+      <c r="EJ101" s="45"/>
+      <c r="EK101" s="45"/>
+      <c r="EL101" s="45"/>
+      <c r="EM101" s="45"/>
+      <c r="EN101" s="45"/>
+      <c r="EO101" s="45"/>
+      <c r="EP101" s="45"/>
+      <c r="EQ101" s="45"/>
+      <c r="ER101" s="45"/>
+      <c r="ES101" s="45"/>
+      <c r="ET101" s="45"/>
+      <c r="EU101" s="45"/>
+      <c r="EV101" s="45"/>
+      <c r="EW101" s="45"/>
+      <c r="EX101" s="45"/>
+      <c r="EY101" s="45"/>
+      <c r="EZ101" s="45"/>
+      <c r="FA101" s="45"/>
+      <c r="FB101" s="45"/>
+      <c r="FC101" s="45"/>
+      <c r="FD101" s="45"/>
+      <c r="FE101" s="45"/>
+      <c r="FF101" s="45"/>
+      <c r="FG101" s="45"/>
+      <c r="FH101" s="45"/>
+      <c r="FI101" s="45"/>
+      <c r="FJ101" s="45"/>
+      <c r="FK101" s="45"/>
+      <c r="FL101" s="45"/>
+      <c r="FM101" s="45"/>
+      <c r="FN101" s="45"/>
+      <c r="FO101" s="45"/>
+      <c r="FP101" s="45"/>
+      <c r="FQ101" s="45"/>
+      <c r="FR101" s="45"/>
+      <c r="FS101" s="45"/>
+      <c r="FT101" s="45"/>
+      <c r="FU101" s="45"/>
+      <c r="FV101" s="45"/>
+      <c r="FW101" s="45"/>
+      <c r="FX101" s="45"/>
+      <c r="FY101" s="45"/>
+      <c r="FZ101" s="45"/>
+      <c r="GA101" s="45"/>
+      <c r="GB101" s="45"/>
+      <c r="GC101" s="45"/>
+      <c r="GD101" s="45"/>
+      <c r="GE101" s="45"/>
+      <c r="GF101" s="45"/>
+      <c r="GG101" s="45"/>
+      <c r="GH101" s="45"/>
+      <c r="GI101" s="45"/>
+      <c r="GJ101" s="45"/>
+      <c r="GK101" s="45"/>
+      <c r="GL101" s="45"/>
+      <c r="GM101" s="45"/>
+      <c r="GN101" s="45"/>
+      <c r="GO101" s="45"/>
+      <c r="GP101" s="45"/>
+      <c r="GQ101" s="45"/>
+      <c r="GR101" s="45"/>
+      <c r="GS101" s="45"/>
+      <c r="GT101" s="45"/>
+      <c r="GU101" s="45"/>
+      <c r="GV101" s="45"/>
+      <c r="GW101" s="45"/>
+      <c r="GX101" s="45"/>
+      <c r="GY101" s="45"/>
+      <c r="GZ101" s="45"/>
+      <c r="HA101" s="45"/>
+      <c r="HB101" s="45"/>
+      <c r="HC101" s="45"/>
+      <c r="HD101" s="45"/>
+      <c r="HE101" s="45"/>
+      <c r="HF101" s="45"/>
+      <c r="HG101" s="45"/>
+      <c r="HH101" s="45"/>
+      <c r="HI101" s="45"/>
+      <c r="HJ101" s="45"/>
+      <c r="HK101" s="45"/>
+      <c r="HL101" s="45"/>
+      <c r="HM101" s="45"/>
+      <c r="HN101" s="45"/>
+      <c r="HO101" s="45"/>
+      <c r="HP101" s="45"/>
+      <c r="HQ101" s="45"/>
+      <c r="HR101" s="45"/>
+      <c r="HS101" s="45"/>
+      <c r="HT101" s="45"/>
+      <c r="HU101" s="45"/>
+      <c r="HV101" s="45"/>
+      <c r="HW101" s="45"/>
+      <c r="HX101" s="45"/>
+      <c r="HY101" s="45"/>
+      <c r="HZ101" s="45"/>
+      <c r="IA101" s="45"/>
+      <c r="IB101" s="45"/>
+      <c r="IC101" s="45"/>
+      <c r="ID101" s="45"/>
+      <c r="IE101" s="45"/>
+      <c r="IF101" s="45"/>
+      <c r="IG101" s="45"/>
+      <c r="IH101" s="45"/>
+      <c r="II101" s="45"/>
+      <c r="IJ101" s="45"/>
+      <c r="IK101" s="45"/>
+      <c r="IL101" s="45"/>
+      <c r="IM101" s="45"/>
+      <c r="IN101" s="45"/>
+      <c r="IO101" s="45"/>
+      <c r="IP101" s="45"/>
+      <c r="IQ101" s="45"/>
+      <c r="IR101" s="45"/>
+      <c r="IS101" s="45"/>
+      <c r="IT101" s="45"/>
+      <c r="IU101" s="45"/>
+      <c r="IV101" s="45"/>
+    </row>
+    <row r="102" spans="1:256" s="49" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="66" t="s">
+        <v>7</v>
+      </c>
+      <c r="B102" s="67" t="s">
+        <v>237</v>
+      </c>
+      <c r="C102" s="67" t="s">
+        <v>58</v>
+      </c>
+      <c r="D102" s="67" t="s">
+        <v>238</v>
+      </c>
+      <c r="E102" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F102" s="68" t="s">
+        <v>75</v>
+      </c>
+      <c r="G102" s="69"/>
+      <c r="H102" s="70"/>
+      <c r="I102" s="70"/>
+      <c r="J102" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="K102" s="47"/>
+      <c r="L102" s="47"/>
+      <c r="M102" s="47"/>
+      <c r="N102" s="47"/>
+      <c r="O102" s="48"/>
+      <c r="P102" s="48"/>
+      <c r="Q102" s="48"/>
+      <c r="R102" s="48"/>
+      <c r="S102" s="48"/>
+      <c r="T102" s="48"/>
+      <c r="U102" s="48"/>
+      <c r="V102" s="48"/>
+      <c r="W102" s="48"/>
+      <c r="X102" s="48"/>
+      <c r="Y102" s="48"/>
+      <c r="Z102" s="48"/>
+      <c r="AA102" s="48"/>
+      <c r="AB102" s="48"/>
+      <c r="AC102" s="48"/>
+      <c r="AD102" s="48"/>
+      <c r="AE102" s="48"/>
+      <c r="AF102" s="48"/>
+      <c r="AG102" s="48"/>
+      <c r="AH102" s="48"/>
+      <c r="AI102" s="48"/>
+      <c r="AJ102" s="48"/>
+      <c r="AK102" s="48"/>
+      <c r="AL102" s="48"/>
+      <c r="AM102" s="48"/>
+      <c r="AN102" s="48"/>
+      <c r="AO102" s="48"/>
+      <c r="AP102" s="48"/>
+      <c r="AQ102" s="48"/>
+      <c r="AR102" s="48"/>
+      <c r="AS102" s="48"/>
+      <c r="AT102" s="48"/>
+      <c r="AU102" s="48"/>
+      <c r="AV102" s="48"/>
+      <c r="AW102" s="48"/>
+      <c r="AX102" s="48"/>
+      <c r="AY102" s="48"/>
+      <c r="AZ102" s="48"/>
+      <c r="BA102" s="48"/>
+      <c r="BB102" s="48"/>
+      <c r="BC102" s="48"/>
+      <c r="BD102" s="48"/>
+      <c r="BE102" s="48"/>
+      <c r="BF102" s="48"/>
+      <c r="BG102" s="48"/>
+      <c r="BH102" s="48"/>
+      <c r="BI102" s="48"/>
+      <c r="BJ102" s="48"/>
+      <c r="BK102" s="48"/>
+      <c r="BL102" s="48"/>
+      <c r="BM102" s="48"/>
+      <c r="BN102" s="48"/>
+      <c r="BO102" s="48"/>
+      <c r="BP102" s="48"/>
+      <c r="BQ102" s="48"/>
+      <c r="BR102" s="48"/>
+      <c r="BS102" s="48"/>
+      <c r="BT102" s="48"/>
+      <c r="BU102" s="48"/>
+      <c r="BV102" s="48"/>
+      <c r="BW102" s="48"/>
+      <c r="BX102" s="48"/>
+      <c r="BY102" s="48"/>
+      <c r="BZ102" s="48"/>
+      <c r="CA102" s="48"/>
+      <c r="CB102" s="48"/>
+      <c r="CC102" s="48"/>
+      <c r="CD102" s="48"/>
+      <c r="CE102" s="48"/>
+      <c r="CF102" s="48"/>
+      <c r="CG102" s="48"/>
+      <c r="CH102" s="48"/>
+      <c r="CI102" s="48"/>
+      <c r="CJ102" s="48"/>
+      <c r="CK102" s="48"/>
+      <c r="CL102" s="48"/>
+      <c r="CM102" s="48"/>
+      <c r="CN102" s="48"/>
+      <c r="CO102" s="48"/>
+      <c r="CP102" s="48"/>
+      <c r="CQ102" s="48"/>
+      <c r="CR102" s="48"/>
+      <c r="CS102" s="48"/>
+      <c r="CT102" s="48"/>
+      <c r="CU102" s="48"/>
+      <c r="CV102" s="48"/>
+      <c r="CW102" s="48"/>
+      <c r="CX102" s="48"/>
+      <c r="CY102" s="48"/>
+      <c r="CZ102" s="48"/>
+      <c r="DA102" s="48"/>
+      <c r="DB102" s="48"/>
+      <c r="DC102" s="48"/>
+      <c r="DD102" s="48"/>
+      <c r="DE102" s="48"/>
+      <c r="DF102" s="48"/>
+      <c r="DG102" s="48"/>
+      <c r="DH102" s="48"/>
+      <c r="DI102" s="48"/>
+      <c r="DJ102" s="48"/>
+      <c r="DK102" s="48"/>
+      <c r="DL102" s="48"/>
+      <c r="DM102" s="48"/>
+      <c r="DN102" s="48"/>
+      <c r="DO102" s="48"/>
+      <c r="DP102" s="48"/>
+      <c r="DQ102" s="48"/>
+      <c r="DR102" s="48"/>
+      <c r="DS102" s="48"/>
+      <c r="DT102" s="48"/>
+      <c r="DU102" s="48"/>
+      <c r="DV102" s="48"/>
+      <c r="DW102" s="48"/>
+      <c r="DX102" s="48"/>
+      <c r="DY102" s="48"/>
+      <c r="DZ102" s="48"/>
+      <c r="EA102" s="48"/>
+      <c r="EB102" s="48"/>
+      <c r="EC102" s="48"/>
+      <c r="ED102" s="48"/>
+      <c r="EE102" s="48"/>
+      <c r="EF102" s="48"/>
+      <c r="EG102" s="48"/>
+      <c r="EH102" s="48"/>
+      <c r="EI102" s="48"/>
+      <c r="EJ102" s="48"/>
+      <c r="EK102" s="48"/>
+      <c r="EL102" s="48"/>
+      <c r="EM102" s="48"/>
+      <c r="EN102" s="48"/>
+      <c r="EO102" s="48"/>
+      <c r="EP102" s="48"/>
+      <c r="EQ102" s="48"/>
+      <c r="ER102" s="48"/>
+      <c r="ES102" s="48"/>
+      <c r="ET102" s="48"/>
+      <c r="EU102" s="48"/>
+      <c r="EV102" s="48"/>
+      <c r="EW102" s="48"/>
+      <c r="EX102" s="48"/>
+      <c r="EY102" s="48"/>
+      <c r="EZ102" s="48"/>
+      <c r="FA102" s="48"/>
+      <c r="FB102" s="48"/>
+      <c r="FC102" s="48"/>
+      <c r="FD102" s="48"/>
+      <c r="FE102" s="48"/>
+      <c r="FF102" s="48"/>
+      <c r="FG102" s="48"/>
+      <c r="FH102" s="48"/>
+      <c r="FI102" s="48"/>
+      <c r="FJ102" s="48"/>
+      <c r="FK102" s="48"/>
+      <c r="FL102" s="48"/>
+      <c r="FM102" s="48"/>
+      <c r="FN102" s="48"/>
+      <c r="FO102" s="48"/>
+      <c r="FP102" s="48"/>
+      <c r="FQ102" s="48"/>
+      <c r="FR102" s="48"/>
+      <c r="FS102" s="48"/>
+      <c r="FT102" s="48"/>
+      <c r="FU102" s="48"/>
+      <c r="FV102" s="48"/>
+      <c r="FW102" s="48"/>
+      <c r="FX102" s="48"/>
+      <c r="FY102" s="48"/>
+      <c r="FZ102" s="48"/>
+      <c r="GA102" s="48"/>
+      <c r="GB102" s="48"/>
+      <c r="GC102" s="48"/>
+      <c r="GD102" s="48"/>
+      <c r="GE102" s="48"/>
+      <c r="GF102" s="48"/>
+      <c r="GG102" s="48"/>
+      <c r="GH102" s="48"/>
+      <c r="GI102" s="48"/>
+      <c r="GJ102" s="48"/>
+      <c r="GK102" s="48"/>
+      <c r="GL102" s="48"/>
+      <c r="GM102" s="48"/>
+      <c r="GN102" s="48"/>
+      <c r="GO102" s="48"/>
+      <c r="GP102" s="48"/>
+      <c r="GQ102" s="48"/>
+      <c r="GR102" s="48"/>
+      <c r="GS102" s="48"/>
+      <c r="GT102" s="48"/>
+      <c r="GU102" s="48"/>
+      <c r="GV102" s="48"/>
+      <c r="GW102" s="48"/>
+      <c r="GX102" s="48"/>
+      <c r="GY102" s="48"/>
+      <c r="GZ102" s="48"/>
+      <c r="HA102" s="48"/>
+      <c r="HB102" s="48"/>
+      <c r="HC102" s="48"/>
+      <c r="HD102" s="48"/>
+      <c r="HE102" s="48"/>
+      <c r="HF102" s="48"/>
+      <c r="HG102" s="48"/>
+      <c r="HH102" s="48"/>
+      <c r="HI102" s="48"/>
+      <c r="HJ102" s="48"/>
+      <c r="HK102" s="48"/>
+      <c r="HL102" s="48"/>
+      <c r="HM102" s="48"/>
+      <c r="HN102" s="48"/>
+      <c r="HO102" s="48"/>
+      <c r="HP102" s="48"/>
+      <c r="HQ102" s="48"/>
+      <c r="HR102" s="48"/>
+      <c r="HS102" s="48"/>
+      <c r="HT102" s="48"/>
+      <c r="HU102" s="48"/>
+      <c r="HV102" s="48"/>
+      <c r="HW102" s="48"/>
+      <c r="HX102" s="48"/>
+      <c r="HY102" s="48"/>
+      <c r="HZ102" s="48"/>
+      <c r="IA102" s="48"/>
+      <c r="IB102" s="48"/>
+      <c r="IC102" s="48"/>
+      <c r="ID102" s="48"/>
+      <c r="IE102" s="48"/>
+      <c r="IF102" s="48"/>
+      <c r="IG102" s="48"/>
+      <c r="IH102" s="48"/>
+      <c r="II102" s="48"/>
+      <c r="IJ102" s="48"/>
+      <c r="IK102" s="48"/>
+      <c r="IL102" s="48"/>
+      <c r="IM102" s="48"/>
+      <c r="IN102" s="48"/>
+      <c r="IO102" s="48"/>
+      <c r="IP102" s="48"/>
+      <c r="IQ102" s="48"/>
+      <c r="IR102" s="48"/>
+      <c r="IS102" s="48"/>
+      <c r="IT102" s="48"/>
+      <c r="IU102" s="48"/>
+      <c r="IV102" s="48"/>
+    </row>
+    <row r="103" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="16"/>
+      <c r="B103" s="16"/>
+      <c r="C103" s="16"/>
+      <c r="D103" s="16"/>
+      <c r="E103" s="16"/>
+      <c r="F103" s="16"/>
+      <c r="G103" s="58"/>
+      <c r="H103" s="59"/>
+      <c r="I103" s="59"/>
       <c r="J103" s="44"/>
       <c r="K103" s="8"/>
       <c r="L103" s="8"/>
       <c r="M103" s="8"/>
       <c r="N103" s="8"/>
     </row>
-    <row r="104" spans="1:256" ht="15.75" customHeight="1">
-      <c r="A104" s="20"/>
-      <c r="B104" s="93" t="s">
-        <v>113</v>
-      </c>
-      <c r="C104" s="94"/>
-      <c r="D104" s="94"/>
-      <c r="E104" s="94"/>
-      <c r="F104" s="95"/>
-      <c r="G104" s="21"/>
-      <c r="H104" s="22"/>
-      <c r="I104" s="22"/>
+    <row r="104" spans="1:256" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="19"/>
+      <c r="B104" s="19"/>
+      <c r="C104" s="19"/>
+      <c r="D104" s="19"/>
+      <c r="E104" s="19"/>
+      <c r="F104" s="19"/>
+      <c r="G104" s="60"/>
+      <c r="H104" s="61"/>
+      <c r="I104" s="61"/>
       <c r="J104" s="44"/>
       <c r="K104" s="8"/>
       <c r="L104" s="8"/>
       <c r="M104" s="8"/>
       <c r="N104" s="8"/>
     </row>
-    <row r="105" spans="1:256" ht="15" customHeight="1">
-      <c r="A105" s="79" t="s">
-        <v>7</v>
-      </c>
-      <c r="B105" s="64" t="s">
-        <v>178</v>
-      </c>
-      <c r="C105" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="D105" s="64" t="s">
-        <v>179</v>
-      </c>
-      <c r="E105" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="F105" s="64" t="s">
-        <v>122</v>
-      </c>
-      <c r="G105" s="52"/>
-      <c r="H105" s="53"/>
-      <c r="I105" s="53">
-        <v>20</v>
-      </c>
+    <row r="105" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="20"/>
+      <c r="B105" s="93" t="s">
+        <v>113</v>
+      </c>
+      <c r="C105" s="94"/>
+      <c r="D105" s="94"/>
+      <c r="E105" s="94"/>
+      <c r="F105" s="95"/>
+      <c r="G105" s="21"/>
+      <c r="H105" s="22"/>
+      <c r="I105" s="22"/>
       <c r="J105" s="44"/>
       <c r="K105" s="8"/>
       <c r="L105" s="8"/>
       <c r="M105" s="8"/>
       <c r="N105" s="8"/>
     </row>
-    <row r="106" spans="1:256" ht="15" customHeight="1">
+    <row r="106" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="79" t="s">
         <v>7</v>
       </c>
       <c r="B106" s="64" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C106" s="64" t="s">
         <v>9</v>
       </c>
       <c r="D106" s="64" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E106" s="64" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F106" s="64" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="G106" s="52"/>
       <c r="H106" s="53"/>
       <c r="I106" s="53">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J106" s="44"/>
       <c r="K106" s="8"/>
@@ -8763,33 +9024,29 @@
       <c r="M106" s="8"/>
       <c r="N106" s="8"/>
     </row>
-    <row r="107" spans="1:256" ht="15" customHeight="1">
-      <c r="A107" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B107" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C107" s="11" t="s">
+    <row r="107" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="79" t="s">
+        <v>7</v>
+      </c>
+      <c r="B107" s="64" t="s">
+        <v>180</v>
+      </c>
+      <c r="C107" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="D107" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="E107" s="11" t="s">
+      <c r="D107" s="64" t="s">
+        <v>181</v>
+      </c>
+      <c r="E107" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="F107" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="G107" s="52">
-        <v>5</v>
-      </c>
-      <c r="H107" s="53">
-        <v>2</v>
-      </c>
+      <c r="F107" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G107" s="52"/>
+      <c r="H107" s="53"/>
       <c r="I107" s="53">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J107" s="44"/>
       <c r="K107" s="8"/>
@@ -8797,29 +9054,33 @@
       <c r="M107" s="8"/>
       <c r="N107" s="8"/>
     </row>
-    <row r="108" spans="1:256" ht="15" customHeight="1">
+    <row r="108" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="10" t="s">
-        <v>123</v>
+        <v>7</v>
       </c>
       <c r="B108" s="11" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C108" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D108" s="11" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E108" s="11" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
       <c r="F108" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="G108" s="52"/>
-      <c r="H108" s="53"/>
+      <c r="G108" s="52">
+        <v>5</v>
+      </c>
+      <c r="H108" s="53">
+        <v>2</v>
+      </c>
       <c r="I108" s="53">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="J108" s="44"/>
       <c r="K108" s="8"/>
@@ -8827,18 +9088,18 @@
       <c r="M108" s="8"/>
       <c r="N108" s="8"/>
     </row>
-    <row r="109" spans="1:256" ht="15" customHeight="1">
+    <row r="109" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="10" t="s">
-        <v>7</v>
+        <v>123</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C109" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D109" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E109" s="11" t="s">
         <v>11</v>
@@ -8846,12 +9107,8 @@
       <c r="F109" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="G109" s="52">
-        <v>5</v>
-      </c>
-      <c r="H109" s="53">
-        <v>3</v>
-      </c>
+      <c r="G109" s="52"/>
+      <c r="H109" s="53"/>
       <c r="I109" s="53">
         <v>35</v>
       </c>
@@ -8861,30 +9118,30 @@
       <c r="M109" s="8"/>
       <c r="N109" s="8"/>
     </row>
-    <row r="110" spans="1:256" ht="15" customHeight="1">
-      <c r="A110" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="B110" s="41" t="s">
-        <v>128</v>
-      </c>
-      <c r="C110" s="41" t="s">
+    <row r="110" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B110" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C110" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D110" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="E110" s="41" t="s">
-        <v>116</v>
-      </c>
-      <c r="F110" s="41" t="s">
-        <v>130</v>
+      <c r="D110" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="E110" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F110" s="11" t="s">
+        <v>122</v>
       </c>
       <c r="G110" s="52">
         <v>5</v>
       </c>
       <c r="H110" s="53">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I110" s="53">
         <v>35</v>
@@ -8895,33 +9152,33 @@
       <c r="M110" s="8"/>
       <c r="N110" s="8"/>
     </row>
-    <row r="111" spans="1:256" ht="15" customHeight="1">
-      <c r="A111" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="B111" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="C111" s="43" t="s">
+    <row r="111" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B111" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="C111" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="D111" s="43" t="s">
-        <v>133</v>
-      </c>
-      <c r="E111" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="F111" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="G111" s="89">
+      <c r="D111" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="E111" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="F111" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="G111" s="52">
         <v>5</v>
       </c>
       <c r="H111" s="53">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I111" s="53">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="J111" s="44"/>
       <c r="K111" s="8"/>
@@ -8929,12 +9186,12 @@
       <c r="M111" s="8"/>
       <c r="N111" s="8"/>
     </row>
-    <row r="112" spans="1:256" ht="15" customHeight="1">
+    <row r="112" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="43" t="s">
         <v>131</v>
       </c>
       <c r="B112" s="43" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C112" s="43" t="s">
         <v>9</v>
@@ -8963,12 +9220,12 @@
       <c r="M112" s="8"/>
       <c r="N112" s="8"/>
     </row>
-    <row r="113" spans="1:14" ht="15" customHeight="1">
+    <row r="113" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="43" t="s">
         <v>131</v>
       </c>
       <c r="B113" s="43" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C113" s="43" t="s">
         <v>9</v>
@@ -8997,7 +9254,7 @@
       <c r="M113" s="8"/>
       <c r="N113" s="8"/>
     </row>
-    <row r="114" spans="1:14" ht="15" customHeight="1">
+    <row r="114" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="43" t="s">
         <v>131</v>
       </c>
@@ -9031,158 +9288,160 @@
       <c r="M114" s="8"/>
       <c r="N114" s="8"/>
     </row>
-    <row r="115" spans="1:14" ht="15" customHeight="1">
+    <row r="115" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="43" t="s">
-        <v>7</v>
+        <v>131</v>
       </c>
       <c r="B115" s="43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C115" s="43" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="D115" s="43" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E115" s="43" t="s">
         <v>11</v>
       </c>
       <c r="F115" s="43" t="s">
-        <v>138</v>
-      </c>
-      <c r="G115" s="75"/>
-      <c r="H115" s="72"/>
-      <c r="I115" s="72"/>
+        <v>122</v>
+      </c>
+      <c r="G115" s="89">
+        <v>5</v>
+      </c>
+      <c r="H115" s="53">
+        <v>5</v>
+      </c>
+      <c r="I115" s="53">
+        <v>20</v>
+      </c>
       <c r="J115" s="44"/>
       <c r="K115" s="8"/>
       <c r="L115" s="8"/>
       <c r="M115" s="8"/>
       <c r="N115" s="8"/>
     </row>
-    <row r="116" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A116" s="90" t="s">
-        <v>7</v>
-      </c>
-      <c r="B116" s="91" t="s">
-        <v>230</v>
-      </c>
-      <c r="C116" s="91" t="s">
+    <row r="116" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B116" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="C116" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="D116" s="91" t="s">
-        <v>231</v>
+      <c r="D116" s="43" t="s">
+        <v>137</v>
       </c>
       <c r="E116" s="43" t="s">
         <v>11</v>
       </c>
       <c r="F116" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="G116" s="56"/>
-      <c r="H116" s="57"/>
-      <c r="I116" s="57"/>
-      <c r="J116" s="44" t="s">
-        <v>190</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="G116" s="75"/>
+      <c r="H116" s="72"/>
+      <c r="I116" s="72"/>
+      <c r="J116" s="44"/>
       <c r="K116" s="8"/>
       <c r="L116" s="8"/>
       <c r="M116" s="8"/>
       <c r="N116" s="8"/>
     </row>
-    <row r="117" spans="1:14" ht="15" customHeight="1">
-      <c r="A117" s="16"/>
-      <c r="B117" s="16"/>
-      <c r="C117" s="16"/>
-      <c r="D117" s="16"/>
-      <c r="E117" s="16"/>
-      <c r="F117" s="16"/>
-      <c r="G117" s="58"/>
-      <c r="H117" s="59"/>
-      <c r="I117" s="59"/>
-      <c r="J117" s="44"/>
+    <row r="117" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="B117" s="91" t="s">
+        <v>230</v>
+      </c>
+      <c r="C117" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="D117" s="91" t="s">
+        <v>231</v>
+      </c>
+      <c r="E117" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="F117" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="G117" s="56"/>
+      <c r="H117" s="57"/>
+      <c r="I117" s="57"/>
+      <c r="J117" s="44" t="s">
+        <v>190</v>
+      </c>
       <c r="K117" s="8"/>
       <c r="L117" s="8"/>
       <c r="M117" s="8"/>
       <c r="N117" s="8"/>
     </row>
-    <row r="118" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A118" s="19"/>
-      <c r="B118" s="19"/>
-      <c r="C118" s="19"/>
-      <c r="D118" s="19"/>
-      <c r="E118" s="23"/>
-      <c r="F118" s="24"/>
-      <c r="G118" s="60"/>
-      <c r="H118" s="61"/>
-      <c r="I118" s="61"/>
+    <row r="118" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="16"/>
+      <c r="B118" s="16"/>
+      <c r="C118" s="16"/>
+      <c r="D118" s="16"/>
+      <c r="E118" s="16"/>
+      <c r="F118" s="16"/>
+      <c r="G118" s="58"/>
+      <c r="H118" s="59"/>
+      <c r="I118" s="59"/>
       <c r="J118" s="44"/>
       <c r="K118" s="8"/>
       <c r="L118" s="8"/>
       <c r="M118" s="8"/>
       <c r="N118" s="8"/>
     </row>
-    <row r="119" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A119" s="20"/>
-      <c r="B119" s="93" t="s">
-        <v>139</v>
-      </c>
-      <c r="C119" s="94"/>
-      <c r="D119" s="94"/>
-      <c r="E119" s="94"/>
-      <c r="F119" s="95"/>
-      <c r="G119" s="21"/>
-      <c r="H119" s="22"/>
-      <c r="I119" s="22"/>
+    <row r="119" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="19"/>
+      <c r="B119" s="19"/>
+      <c r="C119" s="19"/>
+      <c r="D119" s="19"/>
+      <c r="E119" s="23"/>
+      <c r="F119" s="24"/>
+      <c r="G119" s="60"/>
+      <c r="H119" s="61"/>
+      <c r="I119" s="61"/>
       <c r="J119" s="44"/>
       <c r="K119" s="8"/>
       <c r="L119" s="8"/>
       <c r="M119" s="8"/>
       <c r="N119" s="8"/>
     </row>
-    <row r="120" spans="1:14" ht="15" customHeight="1">
-      <c r="A120" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B120" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="C120" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D120" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="E120" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F120" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="G120" s="54">
-        <v>4</v>
-      </c>
-      <c r="H120" s="55">
-        <v>0</v>
-      </c>
-      <c r="I120" s="55"/>
+    <row r="120" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="20"/>
+      <c r="B120" s="93" t="s">
+        <v>139</v>
+      </c>
+      <c r="C120" s="94"/>
+      <c r="D120" s="94"/>
+      <c r="E120" s="94"/>
+      <c r="F120" s="95"/>
+      <c r="G120" s="21"/>
+      <c r="H120" s="22"/>
+      <c r="I120" s="22"/>
       <c r="J120" s="44"/>
       <c r="K120" s="8"/>
       <c r="L120" s="8"/>
       <c r="M120" s="8"/>
       <c r="N120" s="8"/>
     </row>
-    <row r="121" spans="1:14" ht="15" customHeight="1">
+    <row r="121" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B121" s="11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C121" s="11" t="s">
         <v>58</v>
       </c>
       <c r="D121" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E121" s="11" t="s">
         <v>4</v>
@@ -9194,7 +9453,7 @@
         <v>4</v>
       </c>
       <c r="H121" s="55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I121" s="55"/>
       <c r="J121" s="44"/>
@@ -9203,23 +9462,39 @@
       <c r="M121" s="8"/>
       <c r="N121" s="8"/>
     </row>
-    <row r="122" spans="1:14" ht="15" customHeight="1">
-      <c r="A122" s="25"/>
-      <c r="B122" s="12"/>
-      <c r="C122" s="12"/>
-      <c r="D122" s="12"/>
-      <c r="E122" s="12"/>
-      <c r="F122" s="12"/>
-      <c r="G122" s="52"/>
-      <c r="H122" s="53"/>
-      <c r="I122" s="53"/>
+    <row r="122" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B122" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C122" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D122" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="E122" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F122" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="G122" s="54">
+        <v>4</v>
+      </c>
+      <c r="H122" s="55">
+        <v>1</v>
+      </c>
+      <c r="I122" s="55"/>
       <c r="J122" s="44"/>
       <c r="K122" s="8"/>
       <c r="L122" s="8"/>
       <c r="M122" s="8"/>
       <c r="N122" s="8"/>
     </row>
-    <row r="123" spans="1:14" ht="15" customHeight="1">
+    <row r="123" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="25"/>
       <c r="B123" s="12"/>
       <c r="C123" s="12"/>
@@ -9235,7 +9510,7 @@
       <c r="M123" s="8"/>
       <c r="N123" s="8"/>
     </row>
-    <row r="124" spans="1:14" ht="15" customHeight="1">
+    <row r="124" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="25"/>
       <c r="B124" s="12"/>
       <c r="C124" s="12"/>
@@ -9251,97 +9526,83 @@
       <c r="M124" s="8"/>
       <c r="N124" s="8"/>
     </row>
-    <row r="125" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A125" s="14"/>
-      <c r="B125" s="15"/>
-      <c r="C125" s="15"/>
-      <c r="D125" s="15"/>
-      <c r="E125" s="15"/>
-      <c r="F125" s="15"/>
-      <c r="G125" s="56"/>
-      <c r="H125" s="57"/>
-      <c r="I125" s="57"/>
+    <row r="125" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="25"/>
+      <c r="B125" s="12"/>
+      <c r="C125" s="12"/>
+      <c r="D125" s="12"/>
+      <c r="E125" s="12"/>
+      <c r="F125" s="12"/>
+      <c r="G125" s="52"/>
+      <c r="H125" s="53"/>
+      <c r="I125" s="53"/>
       <c r="J125" s="44"/>
       <c r="K125" s="8"/>
       <c r="L125" s="8"/>
       <c r="M125" s="8"/>
       <c r="N125" s="8"/>
     </row>
-    <row r="126" spans="1:14" ht="15" customHeight="1">
-      <c r="A126" s="16"/>
-      <c r="B126" s="16"/>
-      <c r="C126" s="16"/>
-      <c r="D126" s="16"/>
-      <c r="E126" s="16"/>
-      <c r="F126" s="16"/>
-      <c r="G126" s="58"/>
-      <c r="H126" s="59"/>
-      <c r="I126" s="59"/>
+    <row r="126" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="14"/>
+      <c r="B126" s="15"/>
+      <c r="C126" s="15"/>
+      <c r="D126" s="15"/>
+      <c r="E126" s="15"/>
+      <c r="F126" s="15"/>
+      <c r="G126" s="56"/>
+      <c r="H126" s="57"/>
+      <c r="I126" s="57"/>
       <c r="J126" s="44"/>
       <c r="K126" s="8"/>
       <c r="L126" s="8"/>
       <c r="M126" s="8"/>
       <c r="N126" s="8"/>
     </row>
-    <row r="127" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A127" s="19"/>
-      <c r="B127" s="19"/>
-      <c r="C127" s="19"/>
-      <c r="D127" s="19"/>
-      <c r="E127" s="23"/>
-      <c r="F127" s="24"/>
-      <c r="G127" s="60"/>
-      <c r="H127" s="61"/>
-      <c r="I127" s="61"/>
+    <row r="127" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="16"/>
+      <c r="B127" s="16"/>
+      <c r="C127" s="16"/>
+      <c r="D127" s="16"/>
+      <c r="E127" s="16"/>
+      <c r="F127" s="16"/>
+      <c r="G127" s="58"/>
+      <c r="H127" s="59"/>
+      <c r="I127" s="59"/>
       <c r="J127" s="44"/>
       <c r="K127" s="8"/>
       <c r="L127" s="8"/>
       <c r="M127" s="8"/>
       <c r="N127" s="8"/>
     </row>
-    <row r="128" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A128" s="20"/>
-      <c r="B128" s="93" t="s">
-        <v>145</v>
-      </c>
-      <c r="C128" s="94"/>
-      <c r="D128" s="94"/>
-      <c r="E128" s="94"/>
-      <c r="F128" s="95"/>
-      <c r="G128" s="21"/>
-      <c r="H128" s="21"/>
-      <c r="I128" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="J128" s="86"/>
+    <row r="128" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="19"/>
+      <c r="B128" s="19"/>
+      <c r="C128" s="19"/>
+      <c r="D128" s="19"/>
+      <c r="E128" s="23"/>
+      <c r="F128" s="24"/>
+      <c r="G128" s="60"/>
+      <c r="H128" s="61"/>
+      <c r="I128" s="61"/>
+      <c r="J128" s="44"/>
       <c r="K128" s="8"/>
       <c r="L128" s="8"/>
       <c r="M128" s="8"/>
       <c r="N128" s="8"/>
     </row>
-    <row r="129" spans="1:14" ht="15" customHeight="1">
-      <c r="A129" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B129" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="C129" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D129" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="E129" s="28"/>
-      <c r="F129" s="29"/>
-      <c r="G129" s="62">
-        <v>5</v>
-      </c>
-      <c r="H129" s="62">
-        <v>3</v>
-      </c>
-      <c r="I129" s="62">
-        <v>0</v>
+    <row r="129" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="20"/>
+      <c r="B129" s="93" t="s">
+        <v>145</v>
+      </c>
+      <c r="C129" s="94"/>
+      <c r="D129" s="94"/>
+      <c r="E129" s="94"/>
+      <c r="F129" s="95"/>
+      <c r="G129" s="21"/>
+      <c r="H129" s="21"/>
+      <c r="I129" s="21" t="s">
+        <v>146</v>
       </c>
       <c r="J129" s="86"/>
       <c r="K129" s="8"/>
@@ -9349,7 +9610,7 @@
       <c r="M129" s="8"/>
       <c r="N129" s="8"/>
     </row>
-    <row r="130" spans="1:14" ht="15" customHeight="1">
+    <row r="130" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="26" t="s">
         <v>7</v>
       </c>
@@ -9360,7 +9621,7 @@
         <v>9</v>
       </c>
       <c r="D130" s="27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E130" s="28"/>
       <c r="F130" s="29"/>
@@ -9371,7 +9632,7 @@
         <v>3</v>
       </c>
       <c r="I130" s="62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J130" s="86"/>
       <c r="K130" s="8"/>
@@ -9379,7 +9640,7 @@
       <c r="M130" s="8"/>
       <c r="N130" s="8"/>
     </row>
-    <row r="131" spans="1:14" ht="15" customHeight="1">
+    <row r="131" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="26" t="s">
         <v>7</v>
       </c>
@@ -9390,18 +9651,18 @@
         <v>9</v>
       </c>
       <c r="D131" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E131" s="28"/>
-      <c r="F131" s="28"/>
-      <c r="G131" s="63">
+      <c r="F131" s="29"/>
+      <c r="G131" s="62">
         <v>5</v>
       </c>
-      <c r="H131" s="63">
+      <c r="H131" s="62">
         <v>3</v>
       </c>
-      <c r="I131" s="63">
-        <v>2</v>
+      <c r="I131" s="62">
+        <v>1</v>
       </c>
       <c r="J131" s="86"/>
       <c r="K131" s="8"/>
@@ -9409,18 +9670,18 @@
       <c r="M131" s="8"/>
       <c r="N131" s="8"/>
     </row>
-    <row r="132" spans="1:14" ht="15" customHeight="1">
-      <c r="A132" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="B132" s="92" t="s">
-        <v>234</v>
-      </c>
-      <c r="C132" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="D132" s="92" t="s">
-        <v>235</v>
+    <row r="132" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B132" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="C132" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D132" s="27" t="s">
+        <v>149</v>
       </c>
       <c r="E132" s="28"/>
       <c r="F132" s="28"/>
@@ -9428,10 +9689,10 @@
         <v>5</v>
       </c>
       <c r="H132" s="63">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I132" s="63">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J132" s="86"/>
       <c r="K132" s="8"/>
@@ -9439,26 +9700,26 @@
       <c r="M132" s="8"/>
       <c r="N132" s="8"/>
     </row>
-    <row r="133" spans="1:14" ht="15" customHeight="1">
+    <row r="133" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B133" s="28" t="s">
-        <v>173</v>
+      <c r="B133" s="92" t="s">
+        <v>234</v>
       </c>
       <c r="C133" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="D133" s="28" t="s">
-        <v>174</v>
+      <c r="D133" s="92" t="s">
+        <v>235</v>
       </c>
       <c r="E133" s="28"/>
       <c r="F133" s="28"/>
       <c r="G133" s="63">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H133" s="63">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I133" s="63">
         <v>0</v>
@@ -9469,23 +9730,23 @@
       <c r="M133" s="8"/>
       <c r="N133" s="8"/>
     </row>
-    <row r="134" spans="1:14" ht="15.75" customHeight="1">
+    <row r="134" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="30" t="s">
         <v>7</v>
       </c>
       <c r="B134" s="28" t="s">
-        <v>114</v>
+        <v>173</v>
       </c>
       <c r="C134" s="28" t="s">
         <v>58</v>
       </c>
       <c r="D134" s="28" t="s">
-        <v>115</v>
+        <v>174</v>
       </c>
       <c r="E134" s="28"/>
       <c r="F134" s="28"/>
       <c r="G134" s="63">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H134" s="63">
         <v>0</v>
@@ -9499,69 +9760,83 @@
       <c r="M134" s="8"/>
       <c r="N134" s="8"/>
     </row>
-    <row r="135" spans="1:14" ht="15" customHeight="1" thickBot="1">
-      <c r="A135" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="B135" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="C135" s="32" t="s">
+    <row r="135" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B135" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C135" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="D135" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="E135" s="32"/>
-      <c r="F135" s="32"/>
-      <c r="G135" s="78">
+      <c r="D135" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E135" s="28"/>
+      <c r="F135" s="28"/>
+      <c r="G135" s="63">
         <v>5</v>
       </c>
-      <c r="H135" s="78">
-        <v>1</v>
-      </c>
-      <c r="I135" s="78">
+      <c r="H135" s="63">
         <v>0</v>
       </c>
-      <c r="J135" s="44"/>
+      <c r="I135" s="63">
+        <v>0</v>
+      </c>
+      <c r="J135" s="86"/>
       <c r="K135" s="8"/>
       <c r="L135" s="8"/>
       <c r="M135" s="8"/>
       <c r="N135" s="8"/>
     </row>
-    <row r="136" spans="1:14" ht="15" customHeight="1">
-      <c r="A136" s="16"/>
-      <c r="B136" s="16"/>
-      <c r="C136" s="16"/>
-      <c r="D136" s="16"/>
-      <c r="E136" s="33"/>
-      <c r="F136" s="34"/>
-      <c r="G136" s="17"/>
-      <c r="H136" s="18"/>
-      <c r="I136" s="18"/>
+    <row r="136" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B136" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="C136" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D136" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="E136" s="32"/>
+      <c r="F136" s="32"/>
+      <c r="G136" s="78">
+        <v>5</v>
+      </c>
+      <c r="H136" s="78">
+        <v>1</v>
+      </c>
+      <c r="I136" s="78">
+        <v>0</v>
+      </c>
       <c r="J136" s="44"/>
       <c r="K136" s="8"/>
       <c r="L136" s="8"/>
       <c r="M136" s="8"/>
       <c r="N136" s="8"/>
     </row>
-    <row r="137" spans="1:14" ht="15" customHeight="1">
-      <c r="A137" s="35"/>
-      <c r="B137" s="35"/>
-      <c r="C137" s="35"/>
-      <c r="D137" s="35"/>
-      <c r="E137" s="36"/>
-      <c r="F137" s="37"/>
-      <c r="G137" s="38"/>
-      <c r="H137" s="8"/>
-      <c r="I137" s="8"/>
+    <row r="137" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="16"/>
+      <c r="B137" s="16"/>
+      <c r="C137" s="16"/>
+      <c r="D137" s="16"/>
+      <c r="E137" s="33"/>
+      <c r="F137" s="34"/>
+      <c r="G137" s="17"/>
+      <c r="H137" s="18"/>
+      <c r="I137" s="18"/>
       <c r="J137" s="44"/>
       <c r="K137" s="8"/>
       <c r="L137" s="8"/>
       <c r="M137" s="8"/>
       <c r="N137" s="8"/>
     </row>
-    <row r="138" spans="1:14" ht="15" customHeight="1">
+    <row r="138" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="35"/>
       <c r="B138" s="35"/>
       <c r="C138" s="35"/>
@@ -9577,7 +9852,7 @@
       <c r="M138" s="8"/>
       <c r="N138" s="8"/>
     </row>
-    <row r="139" spans="1:14" ht="15" customHeight="1">
+    <row r="139" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="35"/>
       <c r="B139" s="35"/>
       <c r="C139" s="35"/>
@@ -9593,7 +9868,7 @@
       <c r="M139" s="8"/>
       <c r="N139" s="8"/>
     </row>
-    <row r="140" spans="1:14" ht="15" customHeight="1">
+    <row r="140" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="35"/>
       <c r="B140" s="35"/>
       <c r="C140" s="35"/>
@@ -9609,7 +9884,7 @@
       <c r="M140" s="8"/>
       <c r="N140" s="8"/>
     </row>
-    <row r="141" spans="1:14" ht="15" customHeight="1">
+    <row r="141" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="35"/>
       <c r="B141" s="35"/>
       <c r="C141" s="35"/>
@@ -9625,7 +9900,7 @@
       <c r="M141" s="8"/>
       <c r="N141" s="8"/>
     </row>
-    <row r="142" spans="1:14" ht="15" customHeight="1">
+    <row r="142" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="35"/>
       <c r="B142" s="35"/>
       <c r="C142" s="35"/>
@@ -9641,7 +9916,7 @@
       <c r="M142" s="8"/>
       <c r="N142" s="8"/>
     </row>
-    <row r="143" spans="1:14" ht="15" customHeight="1">
+    <row r="143" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="35"/>
       <c r="B143" s="35"/>
       <c r="C143" s="35"/>
@@ -9657,7 +9932,7 @@
       <c r="M143" s="8"/>
       <c r="N143" s="8"/>
     </row>
-    <row r="144" spans="1:14" ht="15" customHeight="1">
+    <row r="144" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="35"/>
       <c r="B144" s="35"/>
       <c r="C144" s="35"/>
@@ -9673,7 +9948,7 @@
       <c r="M144" s="8"/>
       <c r="N144" s="8"/>
     </row>
-    <row r="145" spans="1:14" ht="15" customHeight="1">
+    <row r="145" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="35"/>
       <c r="B145" s="35"/>
       <c r="C145" s="35"/>
@@ -9689,7 +9964,7 @@
       <c r="M145" s="8"/>
       <c r="N145" s="8"/>
     </row>
-    <row r="146" spans="1:14" ht="15" customHeight="1">
+    <row r="146" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="35"/>
       <c r="B146" s="35"/>
       <c r="C146" s="35"/>
@@ -9705,7 +9980,7 @@
       <c r="M146" s="8"/>
       <c r="N146" s="8"/>
     </row>
-    <row r="147" spans="1:14" ht="15" customHeight="1">
+    <row r="147" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="35"/>
       <c r="B147" s="35"/>
       <c r="C147" s="35"/>
@@ -9721,7 +9996,7 @@
       <c r="M147" s="8"/>
       <c r="N147" s="8"/>
     </row>
-    <row r="148" spans="1:14" ht="15" customHeight="1">
+    <row r="148" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="35"/>
       <c r="B148" s="35"/>
       <c r="C148" s="35"/>
@@ -9737,7 +10012,7 @@
       <c r="M148" s="8"/>
       <c r="N148" s="8"/>
     </row>
-    <row r="149" spans="1:14" ht="15" customHeight="1">
+    <row r="149" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="35"/>
       <c r="B149" s="35"/>
       <c r="C149" s="35"/>
@@ -9753,7 +10028,7 @@
       <c r="M149" s="8"/>
       <c r="N149" s="8"/>
     </row>
-    <row r="150" spans="1:14" ht="15" customHeight="1">
+    <row r="150" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="35"/>
       <c r="B150" s="35"/>
       <c r="C150" s="35"/>
@@ -9769,7 +10044,7 @@
       <c r="M150" s="8"/>
       <c r="N150" s="8"/>
     </row>
-    <row r="151" spans="1:14" ht="15" customHeight="1">
+    <row r="151" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="35"/>
       <c r="B151" s="35"/>
       <c r="C151" s="35"/>
@@ -9785,7 +10060,7 @@
       <c r="M151" s="8"/>
       <c r="N151" s="8"/>
     </row>
-    <row r="152" spans="1:14" ht="15" customHeight="1">
+    <row r="152" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="35"/>
       <c r="B152" s="35"/>
       <c r="C152" s="35"/>
@@ -9801,7 +10076,7 @@
       <c r="M152" s="8"/>
       <c r="N152" s="8"/>
     </row>
-    <row r="153" spans="1:14" ht="15" customHeight="1">
+    <row r="153" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="35"/>
       <c r="B153" s="35"/>
       <c r="C153" s="35"/>
@@ -9817,7 +10092,7 @@
       <c r="M153" s="8"/>
       <c r="N153" s="8"/>
     </row>
-    <row r="154" spans="1:14" ht="15" customHeight="1">
+    <row r="154" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="35"/>
       <c r="B154" s="35"/>
       <c r="C154" s="35"/>
@@ -9833,7 +10108,7 @@
       <c r="M154" s="8"/>
       <c r="N154" s="8"/>
     </row>
-    <row r="155" spans="1:14" ht="15" customHeight="1">
+    <row r="155" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="35"/>
       <c r="B155" s="35"/>
       <c r="C155" s="35"/>
@@ -9849,7 +10124,7 @@
       <c r="M155" s="8"/>
       <c r="N155" s="8"/>
     </row>
-    <row r="156" spans="1:14" ht="15" customHeight="1">
+    <row r="156" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="35"/>
       <c r="B156" s="35"/>
       <c r="C156" s="35"/>
@@ -9865,7 +10140,7 @@
       <c r="M156" s="8"/>
       <c r="N156" s="8"/>
     </row>
-    <row r="157" spans="1:14" ht="15" customHeight="1">
+    <row r="157" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="35"/>
       <c r="B157" s="35"/>
       <c r="C157" s="35"/>
@@ -9881,7 +10156,7 @@
       <c r="M157" s="8"/>
       <c r="N157" s="8"/>
     </row>
-    <row r="158" spans="1:14" ht="15" customHeight="1">
+    <row r="158" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="35"/>
       <c r="B158" s="35"/>
       <c r="C158" s="35"/>
@@ -9897,7 +10172,7 @@
       <c r="M158" s="8"/>
       <c r="N158" s="8"/>
     </row>
-    <row r="159" spans="1:14" ht="15" customHeight="1">
+    <row r="159" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="35"/>
       <c r="B159" s="35"/>
       <c r="C159" s="35"/>
@@ -9913,7 +10188,7 @@
       <c r="M159" s="8"/>
       <c r="N159" s="8"/>
     </row>
-    <row r="160" spans="1:14" ht="15" customHeight="1">
+    <row r="160" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="35"/>
       <c r="B160" s="35"/>
       <c r="C160" s="35"/>
@@ -9929,7 +10204,7 @@
       <c r="M160" s="8"/>
       <c r="N160" s="8"/>
     </row>
-    <row r="161" spans="1:14" ht="15" customHeight="1">
+    <row r="161" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="35"/>
       <c r="B161" s="35"/>
       <c r="C161" s="35"/>
@@ -9945,7 +10220,7 @@
       <c r="M161" s="8"/>
       <c r="N161" s="8"/>
     </row>
-    <row r="162" spans="1:14" ht="15" customHeight="1">
+    <row r="162" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="35"/>
       <c r="B162" s="35"/>
       <c r="C162" s="35"/>
@@ -9961,7 +10236,7 @@
       <c r="M162" s="8"/>
       <c r="N162" s="8"/>
     </row>
-    <row r="163" spans="1:14" ht="15" customHeight="1">
+    <row r="163" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="35"/>
       <c r="B163" s="35"/>
       <c r="C163" s="35"/>
@@ -9977,7 +10252,7 @@
       <c r="M163" s="8"/>
       <c r="N163" s="8"/>
     </row>
-    <row r="164" spans="1:14" ht="15" customHeight="1">
+    <row r="164" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="35"/>
       <c r="B164" s="35"/>
       <c r="C164" s="35"/>
@@ -9993,7 +10268,7 @@
       <c r="M164" s="8"/>
       <c r="N164" s="8"/>
     </row>
-    <row r="165" spans="1:14" ht="15" customHeight="1">
+    <row r="165" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="35"/>
       <c r="B165" s="35"/>
       <c r="C165" s="35"/>
@@ -10009,7 +10284,7 @@
       <c r="M165" s="8"/>
       <c r="N165" s="8"/>
     </row>
-    <row r="166" spans="1:14" ht="15" customHeight="1">
+    <row r="166" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="35"/>
       <c r="B166" s="35"/>
       <c r="C166" s="35"/>
@@ -10025,7 +10300,7 @@
       <c r="M166" s="8"/>
       <c r="N166" s="8"/>
     </row>
-    <row r="167" spans="1:14" ht="15" customHeight="1">
+    <row r="167" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="35"/>
       <c r="B167" s="35"/>
       <c r="C167" s="35"/>
@@ -10041,7 +10316,7 @@
       <c r="M167" s="8"/>
       <c r="N167" s="8"/>
     </row>
-    <row r="168" spans="1:14" ht="15" customHeight="1">
+    <row r="168" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="35"/>
       <c r="B168" s="35"/>
       <c r="C168" s="35"/>
@@ -10057,7 +10332,7 @@
       <c r="M168" s="8"/>
       <c r="N168" s="8"/>
     </row>
-    <row r="169" spans="1:14" ht="15" customHeight="1">
+    <row r="169" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="35"/>
       <c r="B169" s="35"/>
       <c r="C169" s="35"/>
@@ -10073,7 +10348,7 @@
       <c r="M169" s="8"/>
       <c r="N169" s="8"/>
     </row>
-    <row r="170" spans="1:14" ht="15" customHeight="1">
+    <row r="170" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="35"/>
       <c r="B170" s="35"/>
       <c r="C170" s="35"/>
@@ -10089,7 +10364,7 @@
       <c r="M170" s="8"/>
       <c r="N170" s="8"/>
     </row>
-    <row r="171" spans="1:14" ht="15" customHeight="1">
+    <row r="171" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="35"/>
       <c r="B171" s="35"/>
       <c r="C171" s="35"/>
@@ -10105,7 +10380,7 @@
       <c r="M171" s="8"/>
       <c r="N171" s="8"/>
     </row>
-    <row r="172" spans="1:14" ht="15" customHeight="1">
+    <row r="172" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="35"/>
       <c r="B172" s="35"/>
       <c r="C172" s="35"/>
@@ -10121,7 +10396,7 @@
       <c r="M172" s="8"/>
       <c r="N172" s="8"/>
     </row>
-    <row r="173" spans="1:14" ht="15" customHeight="1">
+    <row r="173" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="35"/>
       <c r="B173" s="35"/>
       <c r="C173" s="35"/>
@@ -10137,7 +10412,7 @@
       <c r="M173" s="8"/>
       <c r="N173" s="8"/>
     </row>
-    <row r="174" spans="1:14" ht="15" customHeight="1">
+    <row r="174" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="35"/>
       <c r="B174" s="35"/>
       <c r="C174" s="35"/>
@@ -10153,7 +10428,7 @@
       <c r="M174" s="8"/>
       <c r="N174" s="8"/>
     </row>
-    <row r="175" spans="1:14" ht="15" customHeight="1">
+    <row r="175" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="35"/>
       <c r="B175" s="35"/>
       <c r="C175" s="35"/>
@@ -10169,7 +10444,7 @@
       <c r="M175" s="8"/>
       <c r="N175" s="8"/>
     </row>
-    <row r="176" spans="1:14" ht="15" customHeight="1">
+    <row r="176" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="35"/>
       <c r="B176" s="35"/>
       <c r="C176" s="35"/>
@@ -10185,7 +10460,7 @@
       <c r="M176" s="8"/>
       <c r="N176" s="8"/>
     </row>
-    <row r="177" spans="1:14" ht="15" customHeight="1">
+    <row r="177" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="35"/>
       <c r="B177" s="35"/>
       <c r="C177" s="35"/>
@@ -10201,7 +10476,7 @@
       <c r="M177" s="8"/>
       <c r="N177" s="8"/>
     </row>
-    <row r="178" spans="1:14" ht="15" customHeight="1">
+    <row r="178" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="35"/>
       <c r="B178" s="35"/>
       <c r="C178" s="35"/>
@@ -10217,7 +10492,7 @@
       <c r="M178" s="8"/>
       <c r="N178" s="8"/>
     </row>
-    <row r="179" spans="1:14" ht="15" customHeight="1">
+    <row r="179" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="35"/>
       <c r="B179" s="35"/>
       <c r="C179" s="35"/>
@@ -10233,7 +10508,7 @@
       <c r="M179" s="8"/>
       <c r="N179" s="8"/>
     </row>
-    <row r="180" spans="1:14" ht="15" customHeight="1">
+    <row r="180" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="35"/>
       <c r="B180" s="35"/>
       <c r="C180" s="35"/>
@@ -10249,7 +10524,7 @@
       <c r="M180" s="8"/>
       <c r="N180" s="8"/>
     </row>
-    <row r="181" spans="1:14" ht="15" customHeight="1">
+    <row r="181" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="35"/>
       <c r="B181" s="35"/>
       <c r="C181" s="35"/>
@@ -10265,7 +10540,7 @@
       <c r="M181" s="8"/>
       <c r="N181" s="8"/>
     </row>
-    <row r="182" spans="1:14" ht="15" customHeight="1">
+    <row r="182" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="35"/>
       <c r="B182" s="35"/>
       <c r="C182" s="35"/>
@@ -10281,7 +10556,7 @@
       <c r="M182" s="8"/>
       <c r="N182" s="8"/>
     </row>
-    <row r="183" spans="1:14" ht="15" customHeight="1">
+    <row r="183" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="35"/>
       <c r="B183" s="35"/>
       <c r="C183" s="35"/>
@@ -10297,7 +10572,7 @@
       <c r="M183" s="8"/>
       <c r="N183" s="8"/>
     </row>
-    <row r="184" spans="1:14" ht="15" customHeight="1">
+    <row r="184" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="35"/>
       <c r="B184" s="35"/>
       <c r="C184" s="35"/>
@@ -10313,7 +10588,7 @@
       <c r="M184" s="8"/>
       <c r="N184" s="8"/>
     </row>
-    <row r="185" spans="1:14" ht="15" customHeight="1">
+    <row r="185" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="35"/>
       <c r="B185" s="35"/>
       <c r="C185" s="35"/>
@@ -10329,7 +10604,7 @@
       <c r="M185" s="8"/>
       <c r="N185" s="8"/>
     </row>
-    <row r="186" spans="1:14" ht="15" customHeight="1">
+    <row r="186" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="35"/>
       <c r="B186" s="35"/>
       <c r="C186" s="35"/>
@@ -10345,7 +10620,7 @@
       <c r="M186" s="8"/>
       <c r="N186" s="8"/>
     </row>
-    <row r="187" spans="1:14" ht="15" customHeight="1">
+    <row r="187" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="35"/>
       <c r="B187" s="35"/>
       <c r="C187" s="35"/>
@@ -10361,7 +10636,7 @@
       <c r="M187" s="8"/>
       <c r="N187" s="8"/>
     </row>
-    <row r="188" spans="1:14" ht="15" customHeight="1">
+    <row r="188" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="35"/>
       <c r="B188" s="35"/>
       <c r="C188" s="35"/>
@@ -10377,7 +10652,7 @@
       <c r="M188" s="8"/>
       <c r="N188" s="8"/>
     </row>
-    <row r="189" spans="1:14" ht="15" customHeight="1">
+    <row r="189" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="35"/>
       <c r="B189" s="35"/>
       <c r="C189" s="35"/>
@@ -10393,7 +10668,7 @@
       <c r="M189" s="8"/>
       <c r="N189" s="8"/>
     </row>
-    <row r="190" spans="1:14" ht="15" customHeight="1">
+    <row r="190" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="35"/>
       <c r="B190" s="35"/>
       <c r="C190" s="35"/>
@@ -10409,7 +10684,7 @@
       <c r="M190" s="8"/>
       <c r="N190" s="8"/>
     </row>
-    <row r="191" spans="1:14" ht="15" customHeight="1">
+    <row r="191" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="35"/>
       <c r="B191" s="35"/>
       <c r="C191" s="35"/>
@@ -10425,7 +10700,7 @@
       <c r="M191" s="8"/>
       <c r="N191" s="8"/>
     </row>
-    <row r="192" spans="1:14" ht="15" customHeight="1">
+    <row r="192" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="35"/>
       <c r="B192" s="35"/>
       <c r="C192" s="35"/>
@@ -10441,7 +10716,7 @@
       <c r="M192" s="8"/>
       <c r="N192" s="8"/>
     </row>
-    <row r="193" spans="1:14" ht="15" customHeight="1">
+    <row r="193" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="35"/>
       <c r="B193" s="35"/>
       <c r="C193" s="35"/>
@@ -10457,7 +10732,7 @@
       <c r="M193" s="8"/>
       <c r="N193" s="8"/>
     </row>
-    <row r="194" spans="1:14" ht="15" customHeight="1">
+    <row r="194" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="35"/>
       <c r="B194" s="35"/>
       <c r="C194" s="35"/>
@@ -10473,7 +10748,7 @@
       <c r="M194" s="8"/>
       <c r="N194" s="8"/>
     </row>
-    <row r="195" spans="1:14" ht="15" customHeight="1">
+    <row r="195" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="35"/>
       <c r="B195" s="35"/>
       <c r="C195" s="35"/>
@@ -10489,7 +10764,7 @@
       <c r="M195" s="8"/>
       <c r="N195" s="8"/>
     </row>
-    <row r="196" spans="1:14" ht="15" customHeight="1">
+    <row r="196" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="35"/>
       <c r="B196" s="35"/>
       <c r="C196" s="35"/>
@@ -10505,7 +10780,7 @@
       <c r="M196" s="8"/>
       <c r="N196" s="8"/>
     </row>
-    <row r="197" spans="1:14" ht="15" customHeight="1">
+    <row r="197" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="35"/>
       <c r="B197" s="35"/>
       <c r="C197" s="35"/>
@@ -10521,7 +10796,7 @@
       <c r="M197" s="8"/>
       <c r="N197" s="8"/>
     </row>
-    <row r="198" spans="1:14" ht="15" customHeight="1">
+    <row r="198" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="35"/>
       <c r="B198" s="35"/>
       <c r="C198" s="35"/>
@@ -10537,7 +10812,7 @@
       <c r="M198" s="8"/>
       <c r="N198" s="8"/>
     </row>
-    <row r="199" spans="1:14" ht="15" customHeight="1">
+    <row r="199" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="35"/>
       <c r="B199" s="35"/>
       <c r="C199" s="35"/>
@@ -10553,7 +10828,7 @@
       <c r="M199" s="8"/>
       <c r="N199" s="8"/>
     </row>
-    <row r="200" spans="1:14" ht="15" customHeight="1">
+    <row r="200" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="35"/>
       <c r="B200" s="35"/>
       <c r="C200" s="35"/>
@@ -10569,7 +10844,7 @@
       <c r="M200" s="8"/>
       <c r="N200" s="8"/>
     </row>
-    <row r="201" spans="1:14" ht="15" customHeight="1">
+    <row r="201" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="35"/>
       <c r="B201" s="35"/>
       <c r="C201" s="35"/>
@@ -10585,7 +10860,7 @@
       <c r="M201" s="8"/>
       <c r="N201" s="8"/>
     </row>
-    <row r="202" spans="1:14" ht="15" customHeight="1">
+    <row r="202" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="35"/>
       <c r="B202" s="35"/>
       <c r="C202" s="35"/>
@@ -10601,7 +10876,7 @@
       <c r="M202" s="8"/>
       <c r="N202" s="8"/>
     </row>
-    <row r="203" spans="1:14" ht="15" customHeight="1">
+    <row r="203" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="35"/>
       <c r="B203" s="35"/>
       <c r="C203" s="35"/>
@@ -10617,7 +10892,7 @@
       <c r="M203" s="8"/>
       <c r="N203" s="8"/>
     </row>
-    <row r="204" spans="1:14" ht="15" customHeight="1">
+    <row r="204" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="35"/>
       <c r="B204" s="35"/>
       <c r="C204" s="35"/>
@@ -10633,7 +10908,7 @@
       <c r="M204" s="8"/>
       <c r="N204" s="8"/>
     </row>
-    <row r="205" spans="1:14" ht="15" customHeight="1">
+    <row r="205" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="35"/>
       <c r="B205" s="35"/>
       <c r="C205" s="35"/>
@@ -10649,7 +10924,7 @@
       <c r="M205" s="8"/>
       <c r="N205" s="8"/>
     </row>
-    <row r="206" spans="1:14" ht="15" customHeight="1">
+    <row r="206" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="35"/>
       <c r="B206" s="35"/>
       <c r="C206" s="35"/>
@@ -10665,7 +10940,7 @@
       <c r="M206" s="8"/>
       <c r="N206" s="8"/>
     </row>
-    <row r="207" spans="1:14" ht="15" customHeight="1">
+    <row r="207" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="35"/>
       <c r="B207" s="35"/>
       <c r="C207" s="35"/>
@@ -10681,7 +10956,7 @@
       <c r="M207" s="8"/>
       <c r="N207" s="8"/>
     </row>
-    <row r="208" spans="1:14" ht="15" customHeight="1">
+    <row r="208" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="35"/>
       <c r="B208" s="35"/>
       <c r="C208" s="35"/>
@@ -10697,7 +10972,7 @@
       <c r="M208" s="8"/>
       <c r="N208" s="8"/>
     </row>
-    <row r="209" spans="1:14" ht="15" customHeight="1">
+    <row r="209" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="35"/>
       <c r="B209" s="35"/>
       <c r="C209" s="35"/>
@@ -10713,7 +10988,7 @@
       <c r="M209" s="8"/>
       <c r="N209" s="8"/>
     </row>
-    <row r="210" spans="1:14" ht="15" customHeight="1">
+    <row r="210" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="35"/>
       <c r="B210" s="35"/>
       <c r="C210" s="35"/>
@@ -10729,7 +11004,7 @@
       <c r="M210" s="8"/>
       <c r="N210" s="8"/>
     </row>
-    <row r="211" spans="1:14" ht="15" customHeight="1">
+    <row r="211" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="35"/>
       <c r="B211" s="35"/>
       <c r="C211" s="35"/>
@@ -10745,7 +11020,7 @@
       <c r="M211" s="8"/>
       <c r="N211" s="8"/>
     </row>
-    <row r="212" spans="1:14" ht="15" customHeight="1">
+    <row r="212" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="35"/>
       <c r="B212" s="35"/>
       <c r="C212" s="35"/>
@@ -10761,7 +11036,7 @@
       <c r="M212" s="8"/>
       <c r="N212" s="8"/>
     </row>
-    <row r="213" spans="1:14" ht="15" customHeight="1">
+    <row r="213" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="35"/>
       <c r="B213" s="35"/>
       <c r="C213" s="35"/>
@@ -10771,14 +11046,30 @@
       <c r="G213" s="38"/>
       <c r="H213" s="8"/>
       <c r="I213" s="8"/>
+      <c r="J213" s="44"/>
+      <c r="K213" s="8"/>
+      <c r="L213" s="8"/>
+      <c r="M213" s="8"/>
+      <c r="N213" s="8"/>
+    </row>
+    <row r="214" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A214" s="35"/>
+      <c r="B214" s="35"/>
+      <c r="C214" s="35"/>
+      <c r="D214" s="35"/>
+      <c r="E214" s="36"/>
+      <c r="F214" s="37"/>
+      <c r="G214" s="38"/>
+      <c r="H214" s="8"/>
+      <c r="I214" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B119:F119"/>
-    <mergeCell ref="B104:F104"/>
+    <mergeCell ref="B120:F120"/>
+    <mergeCell ref="B105:F105"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B128:F128"/>
+    <mergeCell ref="B129:F129"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740200000000005" bottom="0.78740200000000005" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>